<commit_message>
H2 updated - gas based h2 turned off for now.
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_SUP_Hydrogen.xlsx
+++ b/SubRes_TMPL/SubRES_SUP_Hydrogen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EEB239-D33D-4D50-9E06-F0C71F43DC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A88EE2-E522-4B2B-BE35-6C8DAFD1972F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="26610" windowHeight="13740" activeTab="2" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="7" r:id="rId1"/>
@@ -1184,7 +1184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="838">
   <si>
     <t>Document type:</t>
   </si>
@@ -5445,6 +5445,9 @@
   </si>
   <si>
     <t>*Storage</t>
+  </si>
+  <si>
+    <t>ENV_ACT~CH4C</t>
   </si>
 </sst>
 </file>
@@ -7309,93 +7312,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="4" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="15" fillId="21" borderId="27" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="81" fillId="0" borderId="28" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -7490,6 +7406,93 @@
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="14" applyFill="1"/>
     <xf numFmtId="165" fontId="78" fillId="0" borderId="30" xfId="14" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -15900,6 +15903,7 @@
       <sheetName val="TS XEmiss"/>
       <sheetName val="TID XEmiss"/>
       <sheetName val="ExchangeRateDetail"/>
+      <sheetName val="Deflator"/>
       <sheetName val="SUPRES"/>
       <sheetName val="ITEMS_XFEmiss"/>
       <sheetName val="TS XFEmiss"/>
@@ -16339,6 +16343,14 @@
             <v>Upstream</v>
           </cell>
         </row>
+        <row r="56">
+          <cell r="B56"/>
+          <cell r="C56"/>
+        </row>
+        <row r="57">
+          <cell r="B57"/>
+          <cell r="C57"/>
+        </row>
       </sheetData>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4">
@@ -16446,6 +16458,7 @@
       <sheetData sheetId="64"/>
       <sheetData sheetId="65"/>
       <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -17476,12 +17489,12 @@
       <c r="Z15" s="17"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="303" t="s">
+      <c r="A16" s="344" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="303"/>
-      <c r="C16" s="303"/>
-      <c r="D16" s="303"/>
+      <c r="B16" s="344"/>
+      <c r="C16" s="344"/>
+      <c r="D16" s="344"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="19"/>
@@ -17565,11 +17578,11 @@
       <c r="A19" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="302" t="s">
+      <c r="B19" s="343" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="302"/>
-      <c r="D19" s="302"/>
+      <c r="C19" s="343"/>
+      <c r="D19" s="343"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="25"/>
@@ -17597,11 +17610,11 @@
       <c r="A20" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="302" t="s">
+      <c r="B20" s="343" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="302"/>
-      <c r="D20" s="302"/>
+      <c r="C20" s="343"/>
+      <c r="D20" s="343"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="25"/>
@@ -17689,11 +17702,11 @@
       <c r="A23" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="302" t="s">
+      <c r="B23" s="343" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="302"/>
-      <c r="D23" s="302"/>
+      <c r="C23" s="343"/>
+      <c r="D23" s="343"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -17777,9 +17790,9 @@
       <c r="A26" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="302"/>
-      <c r="C26" s="302"/>
-      <c r="D26" s="302"/>
+      <c r="B26" s="343"/>
+      <c r="C26" s="343"/>
+      <c r="D26" s="343"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -17895,9 +17908,9 @@
       <c r="A30" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="304"/>
-      <c r="C30" s="302"/>
-      <c r="D30" s="302"/>
+      <c r="B30" s="345"/>
+      <c r="C30" s="343"/>
+      <c r="D30" s="343"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28"/>
       <c r="G30" s="17"/>
@@ -17925,11 +17938,11 @@
       <c r="A31" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="302" t="s">
+      <c r="B31" s="343" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="302"/>
-      <c r="D31" s="302"/>
+      <c r="C31" s="343"/>
+      <c r="D31" s="343"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="17"/>
@@ -20623,16 +20636,16 @@
       <c r="K6" s="204" t="s">
         <v>546</v>
       </c>
-      <c r="L6" s="305" t="s">
+      <c r="L6" s="346" t="s">
         <v>545</v>
       </c>
-      <c r="M6" s="306"/>
-      <c r="N6" s="307"/>
-      <c r="O6" s="305" t="s">
+      <c r="M6" s="347"/>
+      <c r="N6" s="348"/>
+      <c r="O6" s="346" t="s">
         <v>484</v>
       </c>
-      <c r="P6" s="306"/>
-      <c r="Q6" s="307"/>
+      <c r="P6" s="347"/>
+      <c r="Q6" s="348"/>
       <c r="X6" s="144" t="s">
         <v>544</v>
       </c>
@@ -20644,9 +20657,9 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="I7" s="313"/>
-      <c r="J7" s="313"/>
-      <c r="K7" s="313"/>
+      <c r="I7" s="354"/>
+      <c r="J7" s="354"/>
+      <c r="K7" s="354"/>
       <c r="L7" s="203">
         <v>2000</v>
       </c>
@@ -20724,15 +20737,15 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="314" t="s">
+      <c r="A9" s="355" t="s">
         <v>536</v>
       </c>
-      <c r="B9" s="314"/>
-      <c r="C9" s="314"/>
-      <c r="D9" s="314"/>
-      <c r="E9" s="314"/>
-      <c r="F9" s="314"/>
-      <c r="G9" s="314"/>
+      <c r="B9" s="355"/>
+      <c r="C9" s="355"/>
+      <c r="D9" s="355"/>
+      <c r="E9" s="355"/>
+      <c r="F9" s="355"/>
+      <c r="G9" s="355"/>
       <c r="I9" s="200" t="s">
         <v>409</v>
       </c>
@@ -21308,33 +21321,33 @@
       <c r="K26" s="150" t="s">
         <v>486</v>
       </c>
-      <c r="L26" s="312" t="s">
+      <c r="L26" s="353" t="s">
         <v>485</v>
       </c>
-      <c r="M26" s="312"/>
-      <c r="N26" s="312"/>
-      <c r="O26" s="312" t="s">
+      <c r="M26" s="353"/>
+      <c r="N26" s="353"/>
+      <c r="O26" s="353" t="s">
         <v>484</v>
       </c>
-      <c r="P26" s="312"/>
-      <c r="Q26" s="312"/>
-      <c r="R26" s="312" t="s">
+      <c r="P26" s="353"/>
+      <c r="Q26" s="353"/>
+      <c r="R26" s="353" t="s">
         <v>483</v>
       </c>
-      <c r="S26" s="312"/>
-      <c r="T26" s="312"/>
-      <c r="U26" s="322" t="s">
+      <c r="S26" s="353"/>
+      <c r="T26" s="353"/>
+      <c r="U26" s="363" t="s">
         <v>414</v>
       </c>
-      <c r="V26" s="322"/>
+      <c r="V26" s="363"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>482</v>
       </c>
-      <c r="I27" s="318"/>
-      <c r="J27" s="318"/>
-      <c r="K27" s="318"/>
+      <c r="I27" s="359"/>
+      <c r="J27" s="359"/>
+      <c r="K27" s="359"/>
       <c r="L27" s="188">
         <v>2000</v>
       </c>
@@ -21561,11 +21574,11 @@
       <c r="C31" s="145" t="s">
         <v>398</v>
       </c>
-      <c r="D31" s="319" t="s">
+      <c r="D31" s="360" t="s">
         <v>396</v>
       </c>
-      <c r="E31" s="319"/>
-      <c r="F31" s="319"/>
+      <c r="E31" s="360"/>
+      <c r="F31" s="360"/>
       <c r="I31" s="141" t="s">
         <v>407</v>
       </c>
@@ -21644,11 +21657,11 @@
       <c r="C32" s="182" t="s">
         <v>433</v>
       </c>
-      <c r="D32" s="320" t="s">
+      <c r="D32" s="361" t="s">
         <v>435</v>
       </c>
-      <c r="E32" s="320"/>
-      <c r="F32" s="320"/>
+      <c r="E32" s="361"/>
+      <c r="F32" s="361"/>
       <c r="I32" s="141" t="s">
         <v>407</v>
       </c>
@@ -21728,11 +21741,11 @@
       <c r="C33" s="182" t="s">
         <v>433</v>
       </c>
-      <c r="D33" s="321" t="s">
+      <c r="D33" s="362" t="s">
         <v>475</v>
       </c>
-      <c r="E33" s="321"/>
-      <c r="F33" s="321"/>
+      <c r="E33" s="362"/>
+      <c r="F33" s="362"/>
       <c r="I33" s="141" t="s">
         <v>403</v>
       </c>
@@ -21812,11 +21825,11 @@
       <c r="C34" s="182" t="s">
         <v>433</v>
       </c>
-      <c r="D34" s="321" t="s">
+      <c r="D34" s="362" t="s">
         <v>472</v>
       </c>
-      <c r="E34" s="321"/>
-      <c r="F34" s="321"/>
+      <c r="E34" s="362"/>
+      <c r="F34" s="362"/>
       <c r="I34" s="141" t="s">
         <v>403</v>
       </c>
@@ -22378,20 +22391,20 @@
       <c r="N45" s="134"/>
     </row>
     <row r="46" spans="1:35" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="308" t="s">
+      <c r="I46" s="349" t="s">
         <v>419</v>
       </c>
-      <c r="J46" s="308" t="s">
+      <c r="J46" s="349" t="s">
         <v>418</v>
       </c>
-      <c r="K46" s="310" t="s">
+      <c r="K46" s="351" t="s">
         <v>417</v>
       </c>
-      <c r="L46" s="315" t="s">
+      <c r="L46" s="356" t="s">
         <v>448</v>
       </c>
-      <c r="M46" s="316"/>
-      <c r="N46" s="317"/>
+      <c r="M46" s="357"/>
+      <c r="N46" s="358"/>
       <c r="R46" t="s">
         <v>447</v>
       </c>
@@ -22400,9 +22413,9 @@
       <c r="A47" s="159" t="s">
         <v>446</v>
       </c>
-      <c r="I47" s="309"/>
-      <c r="J47" s="309"/>
-      <c r="K47" s="311"/>
+      <c r="I47" s="350"/>
+      <c r="J47" s="350"/>
+      <c r="K47" s="352"/>
       <c r="L47" s="149">
         <v>2000</v>
       </c>
@@ -22437,15 +22450,15 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="314" t="s">
+      <c r="A49" s="355" t="s">
         <v>445</v>
       </c>
-      <c r="B49" s="314"/>
-      <c r="C49" s="314"/>
-      <c r="D49" s="314"/>
-      <c r="E49" s="314"/>
-      <c r="F49" s="314"/>
-      <c r="G49" s="314"/>
+      <c r="B49" s="355"/>
+      <c r="C49" s="355"/>
+      <c r="D49" s="355"/>
+      <c r="E49" s="355"/>
+      <c r="F49" s="355"/>
+      <c r="G49" s="355"/>
       <c r="I49" s="141" t="s">
         <v>444</v>
       </c>
@@ -22919,34 +22932,34 @@
       <c r="A67" s="151" t="s">
         <v>420</v>
       </c>
-      <c r="I67" s="323" t="s">
+      <c r="I67" s="364" t="s">
         <v>419</v>
       </c>
-      <c r="J67" s="323" t="s">
+      <c r="J67" s="364" t="s">
         <v>418</v>
       </c>
-      <c r="K67" s="324" t="s">
+      <c r="K67" s="365" t="s">
         <v>417</v>
       </c>
-      <c r="L67" s="325" t="s">
+      <c r="L67" s="366" t="s">
         <v>416</v>
       </c>
-      <c r="M67" s="312"/>
-      <c r="N67" s="312"/>
-      <c r="O67" s="325" t="s">
+      <c r="M67" s="353"/>
+      <c r="N67" s="353"/>
+      <c r="O67" s="366" t="s">
         <v>415</v>
       </c>
-      <c r="P67" s="312"/>
-      <c r="Q67" s="312"/>
-      <c r="R67" s="322" t="s">
+      <c r="P67" s="353"/>
+      <c r="Q67" s="353"/>
+      <c r="R67" s="363" t="s">
         <v>414</v>
       </c>
-      <c r="S67" s="322"/>
+      <c r="S67" s="363"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I68" s="323"/>
-      <c r="J68" s="323"/>
-      <c r="K68" s="324"/>
+      <c r="I68" s="364"/>
+      <c r="J68" s="364"/>
+      <c r="K68" s="365"/>
       <c r="L68" s="149">
         <v>2000</v>
       </c>
@@ -23623,14 +23636,14 @@
       <c r="I87" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="J87" s="329" t="s">
+      <c r="J87" s="370" t="s">
         <v>373</v>
       </c>
-      <c r="K87" s="329"/>
-      <c r="L87" s="329" t="s">
+      <c r="K87" s="370"/>
+      <c r="L87" s="370" t="s">
         <v>372</v>
       </c>
-      <c r="M87" s="329"/>
+      <c r="M87" s="370"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -24306,16 +24319,16 @@
       <c r="J123" s="113" t="s">
         <v>327</v>
       </c>
-      <c r="K123" s="326" t="s">
+      <c r="K123" s="367" t="s">
         <v>326</v>
       </c>
-      <c r="L123" s="327"/>
-      <c r="M123" s="328"/>
-      <c r="N123" s="326" t="s">
+      <c r="L123" s="368"/>
+      <c r="M123" s="369"/>
+      <c r="N123" s="367" t="s">
         <v>325</v>
       </c>
-      <c r="O123" s="327"/>
-      <c r="P123" s="328"/>
+      <c r="O123" s="368"/>
+      <c r="P123" s="369"/>
       <c r="Q123" s="114"/>
     </row>
     <row r="124" spans="9:17" x14ac:dyDescent="0.25">
@@ -24398,61 +24411,61 @@
       <c r="Q126" s="114"/>
     </row>
     <row r="128" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I128" s="314" t="s">
+      <c r="I128" s="355" t="s">
         <v>321</v>
       </c>
-      <c r="J128" s="314"/>
-      <c r="K128" s="314"/>
-      <c r="L128" s="314"/>
-      <c r="M128" s="314"/>
-      <c r="N128" s="314"/>
-      <c r="O128" s="314"/>
-      <c r="P128" s="314"/>
-      <c r="Q128" s="314"/>
+      <c r="J128" s="355"/>
+      <c r="K128" s="355"/>
+      <c r="L128" s="355"/>
+      <c r="M128" s="355"/>
+      <c r="N128" s="355"/>
+      <c r="O128" s="355"/>
+      <c r="P128" s="355"/>
+      <c r="Q128" s="355"/>
     </row>
     <row r="129" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I129" s="314"/>
-      <c r="J129" s="314"/>
-      <c r="K129" s="314"/>
-      <c r="L129" s="314"/>
-      <c r="M129" s="314"/>
-      <c r="N129" s="314"/>
-      <c r="O129" s="314"/>
-      <c r="P129" s="314"/>
-      <c r="Q129" s="314"/>
+      <c r="I129" s="355"/>
+      <c r="J129" s="355"/>
+      <c r="K129" s="355"/>
+      <c r="L129" s="355"/>
+      <c r="M129" s="355"/>
+      <c r="N129" s="355"/>
+      <c r="O129" s="355"/>
+      <c r="P129" s="355"/>
+      <c r="Q129" s="355"/>
     </row>
     <row r="130" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I130" s="314"/>
-      <c r="J130" s="314"/>
-      <c r="K130" s="314"/>
-      <c r="L130" s="314"/>
-      <c r="M130" s="314"/>
-      <c r="N130" s="314"/>
-      <c r="O130" s="314"/>
-      <c r="P130" s="314"/>
-      <c r="Q130" s="314"/>
+      <c r="I130" s="355"/>
+      <c r="J130" s="355"/>
+      <c r="K130" s="355"/>
+      <c r="L130" s="355"/>
+      <c r="M130" s="355"/>
+      <c r="N130" s="355"/>
+      <c r="O130" s="355"/>
+      <c r="P130" s="355"/>
+      <c r="Q130" s="355"/>
     </row>
     <row r="131" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I131" s="314"/>
-      <c r="J131" s="314"/>
-      <c r="K131" s="314"/>
-      <c r="L131" s="314"/>
-      <c r="M131" s="314"/>
-      <c r="N131" s="314"/>
-      <c r="O131" s="314"/>
-      <c r="P131" s="314"/>
-      <c r="Q131" s="314"/>
+      <c r="I131" s="355"/>
+      <c r="J131" s="355"/>
+      <c r="K131" s="355"/>
+      <c r="L131" s="355"/>
+      <c r="M131" s="355"/>
+      <c r="N131" s="355"/>
+      <c r="O131" s="355"/>
+      <c r="P131" s="355"/>
+      <c r="Q131" s="355"/>
     </row>
     <row r="132" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I132" s="314"/>
-      <c r="J132" s="314"/>
-      <c r="K132" s="314"/>
-      <c r="L132" s="314"/>
-      <c r="M132" s="314"/>
-      <c r="N132" s="314"/>
-      <c r="O132" s="314"/>
-      <c r="P132" s="314"/>
-      <c r="Q132" s="314"/>
+      <c r="I132" s="355"/>
+      <c r="J132" s="355"/>
+      <c r="K132" s="355"/>
+      <c r="L132" s="355"/>
+      <c r="M132" s="355"/>
+      <c r="N132" s="355"/>
+      <c r="O132" s="355"/>
+      <c r="P132" s="355"/>
+      <c r="Q132" s="355"/>
     </row>
     <row r="134" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I134" s="114" t="s">
@@ -25343,7 +25356,7 @@
         <f>J5</f>
         <v>2050</v>
       </c>
-      <c r="K40" s="330" t="s">
+      <c r="K40" s="371" t="s">
         <v>577</v>
       </c>
       <c r="L40" s="60" t="s">
@@ -25386,7 +25399,7 @@
         <f>INDEX(L41:M41,MATCH($J$43,$L$43:$M$43,0))</f>
         <v>390.90909090909093</v>
       </c>
-      <c r="K41" s="330"/>
+      <c r="K41" s="371"/>
       <c r="L41" s="144">
         <v>200</v>
       </c>
@@ -25425,7 +25438,7 @@
         <f>INDEX(L42:M42,MATCH($J$43,$L$43:$M$43,0))</f>
         <v>277.77777777777777</v>
       </c>
-      <c r="K42" s="330"/>
+      <c r="K42" s="371"/>
       <c r="L42" s="144">
         <v>200</v>
       </c>
@@ -30307,511 +30320,511 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="366" t="s">
+      <c r="A1" s="337" t="s">
         <v>808</v>
       </c>
-      <c r="B1" s="366">
+      <c r="B1" s="337">
         <v>1991</v>
       </c>
-      <c r="C1" s="366">
+      <c r="C1" s="337">
         <v>1992</v>
       </c>
-      <c r="D1" s="366">
+      <c r="D1" s="337">
         <v>1993</v>
       </c>
-      <c r="E1" s="366">
+      <c r="E1" s="337">
         <v>1994</v>
       </c>
-      <c r="F1" s="366">
+      <c r="F1" s="337">
         <v>1995</v>
       </c>
-      <c r="G1" s="366">
+      <c r="G1" s="337">
         <v>1996</v>
       </c>
-      <c r="H1" s="366">
+      <c r="H1" s="337">
         <v>1997</v>
       </c>
-      <c r="I1" s="366">
+      <c r="I1" s="337">
         <v>1998</v>
       </c>
-      <c r="J1" s="366">
+      <c r="J1" s="337">
         <v>1999</v>
       </c>
-      <c r="K1" s="366">
+      <c r="K1" s="337">
         <v>2000</v>
       </c>
-      <c r="L1" s="366">
+      <c r="L1" s="337">
         <v>2001</v>
       </c>
-      <c r="M1" s="366">
+      <c r="M1" s="337">
         <v>2002</v>
       </c>
-      <c r="N1" s="366">
+      <c r="N1" s="337">
         <v>2003</v>
       </c>
-      <c r="O1" s="366">
+      <c r="O1" s="337">
         <v>2004</v>
       </c>
-      <c r="P1" s="366">
+      <c r="P1" s="337">
         <v>2005</v>
       </c>
-      <c r="Q1" s="366">
+      <c r="Q1" s="337">
         <v>2006</v>
       </c>
-      <c r="R1" s="366">
+      <c r="R1" s="337">
         <v>2007</v>
       </c>
-      <c r="S1" s="366">
+      <c r="S1" s="337">
         <v>2008</v>
       </c>
-      <c r="T1" s="366">
+      <c r="T1" s="337">
         <v>2009</v>
       </c>
-      <c r="U1" s="365">
+      <c r="U1" s="336">
         <v>2010</v>
       </c>
-      <c r="V1" s="365">
+      <c r="V1" s="336">
         <v>2011</v>
       </c>
-      <c r="W1" s="365">
+      <c r="W1" s="336">
         <v>2012</v>
       </c>
-      <c r="X1" s="364">
+      <c r="X1" s="335">
         <v>2013</v>
       </c>
-      <c r="Y1" s="364">
+      <c r="Y1" s="335">
         <v>2014</v>
       </c>
-      <c r="Z1" s="364">
+      <c r="Z1" s="335">
         <v>2015</v>
       </c>
-      <c r="AA1" s="364">
+      <c r="AA1" s="335">
         <v>2016</v>
       </c>
-      <c r="AB1" s="363">
+      <c r="AB1" s="334">
         <v>2017</v>
       </c>
-      <c r="AC1" s="363">
+      <c r="AC1" s="334">
         <v>2018</v>
       </c>
-      <c r="AD1" s="363">
+      <c r="AD1" s="334">
         <v>2019</v>
       </c>
-      <c r="AE1" s="350">
+      <c r="AE1" s="321">
         <v>2020</v>
       </c>
-      <c r="AF1" s="350">
+      <c r="AF1" s="321">
         <v>2021</v>
       </c>
-      <c r="AG1" s="350"/>
-      <c r="AH1" s="362" t="s">
+      <c r="AG1" s="321"/>
+      <c r="AH1" s="333" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="361" t="s">
+      <c r="A2" s="332" t="s">
         <v>785</v>
       </c>
-      <c r="B2" s="360">
+      <c r="B2" s="331">
         <v>15.727008694067001</v>
       </c>
-      <c r="C2" s="360">
+      <c r="C2" s="331">
         <v>14.5711517216375</v>
       </c>
-      <c r="D2" s="360">
+      <c r="D2" s="331">
         <v>13.0875688743451</v>
       </c>
-      <c r="E2" s="360">
+      <c r="E2" s="331">
         <v>9.5940101543789797</v>
       </c>
-      <c r="F2" s="360">
+      <c r="F2" s="331">
         <v>10.250325952765699</v>
       </c>
-      <c r="G2" s="359">
+      <c r="G2" s="330">
         <v>7.9057626177225204</v>
       </c>
-      <c r="H2" s="359">
+      <c r="H2" s="330">
         <v>7.9871533674518798</v>
       </c>
-      <c r="I2" s="359">
+      <c r="I2" s="330">
         <v>7.7873391569621004</v>
       </c>
-      <c r="J2" s="359">
+      <c r="J2" s="330">
         <v>7.0278247472558499</v>
       </c>
-      <c r="K2" s="359">
+      <c r="K2" s="330">
         <v>8.7963222595021993</v>
       </c>
-      <c r="L2" s="359">
+      <c r="L2" s="330">
         <v>7.6417362147513304</v>
       </c>
-      <c r="M2" s="359">
+      <c r="M2" s="330">
         <v>12.205405688193901</v>
       </c>
-      <c r="N2" s="359">
+      <c r="N2" s="330">
         <v>5.7936025975283902</v>
       </c>
-      <c r="O2" s="359">
+      <c r="O2" s="330">
         <v>6.5271139772024496</v>
       </c>
-      <c r="P2" s="359">
+      <c r="P2" s="330">
         <v>5.4490666230227598</v>
       </c>
-      <c r="Q2" s="359">
+      <c r="Q2" s="330">
         <v>6.2741537708994999</v>
       </c>
-      <c r="R2" s="359">
+      <c r="R2" s="330">
         <v>8.8492898126298094</v>
       </c>
-      <c r="S2" s="359">
+      <c r="S2" s="330">
         <v>8.8315688644124695</v>
       </c>
-      <c r="T2" s="359">
+      <c r="T2" s="330">
         <v>7.5045113457487203</v>
       </c>
-      <c r="U2" s="359">
+      <c r="U2" s="330">
         <v>6.3510267905241404</v>
       </c>
-      <c r="V2" s="359">
+      <c r="V2" s="330">
         <v>6.6517827868979502</v>
       </c>
-      <c r="W2" s="359">
+      <c r="W2" s="330">
         <v>5.5122264718124399</v>
       </c>
-      <c r="X2" s="359">
+      <c r="X2" s="330">
         <v>5.9856351455896997</v>
       </c>
-      <c r="Y2" s="359">
+      <c r="Y2" s="330">
         <v>5.79552879780148</v>
       </c>
-      <c r="Z2" s="359">
+      <c r="Z2" s="330">
         <v>4.5454545454545414</v>
       </c>
-      <c r="AA2" s="359">
+      <c r="AA2" s="330">
         <v>6.3405797101449224</v>
       </c>
-      <c r="AB2" s="358">
+      <c r="AB2" s="329">
         <v>5.2725724020443065</v>
       </c>
-      <c r="AC2" s="358">
+      <c r="AC2" s="329">
         <v>4.6201148960271832</v>
       </c>
-      <c r="AD2" s="358">
+      <c r="AD2" s="329">
         <v>4.1299303944315469</v>
       </c>
-      <c r="AE2" s="350"/>
-      <c r="AF2" s="350"/>
-      <c r="AG2" s="350"/>
-      <c r="AH2" s="350"/>
+      <c r="AE2" s="321"/>
+      <c r="AF2" s="321"/>
+      <c r="AG2" s="321"/>
+      <c r="AH2" s="321"/>
     </row>
     <row r="3" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="341">
+      <c r="A3" s="312">
         <f>B12</f>
         <v>2015</v>
       </c>
-      <c r="B3" s="340">
-        <f>IF(B1=$A$3,1,IF(B1&lt;$A3,C3/(1+C2/100),A3*(B2/100+1)))</f>
+      <c r="B3" s="311">
+        <f t="shared" ref="B3:Y3" si="0">IF(B1=$A$3,1,IF(B1&lt;$A3,C3/(1+C2/100),A3*(B2/100+1)))</f>
         <v>0.16025960579724249</v>
       </c>
-      <c r="C3" s="340">
-        <f>IF(C1=$A$3,1,IF(C1&lt;$A3,D3/(1+D2/100),B3*(C2/100+1)))</f>
+      <c r="C3" s="311">
+        <f t="shared" si="0"/>
         <v>0.18361127610645686</v>
       </c>
-      <c r="D3" s="340">
-        <f>IF(D1=$A$3,1,IF(D1&lt;$A3,E3/(1+E2/100),C3*(D2/100+1)))</f>
+      <c r="D3" s="311">
+        <f t="shared" si="0"/>
         <v>0.20764152832795335</v>
       </c>
-      <c r="E3" s="340">
-        <f>IF(E1=$A$3,1,IF(E1&lt;$A3,F3/(1+F2/100),D3*(E2/100+1)))</f>
+      <c r="E3" s="311">
+        <f t="shared" si="0"/>
         <v>0.22756267764044488</v>
       </c>
-      <c r="F3" s="340">
-        <f>IF(F1=$A$3,1,IF(F1&lt;$A3,G3/(1+G2/100),E3*(F2/100+1)))</f>
+      <c r="F3" s="311">
+        <f t="shared" si="0"/>
         <v>0.25088859384543194</v>
       </c>
-      <c r="G3" s="340">
-        <f>IF(G1=$A$3,1,IF(G1&lt;$A3,H3/(1+H2/100),F3*(G2/100+1)))</f>
+      <c r="G3" s="311">
+        <f t="shared" si="0"/>
         <v>0.27072325050979379</v>
       </c>
-      <c r="H3" s="340">
-        <f>IF(H1=$A$3,1,IF(H1&lt;$A3,I3/(1+I2/100),G3*(H2/100+1)))</f>
+      <c r="H3" s="311">
+        <f t="shared" si="0"/>
         <v>0.29234633172936197</v>
       </c>
-      <c r="I3" s="340">
-        <f>IF(I1=$A$3,1,IF(I1&lt;$A3,J3/(1+J2/100),H3*(I2/100+1)))</f>
+      <c r="I3" s="311">
+        <f t="shared" si="0"/>
         <v>0.31511233209406492</v>
       </c>
-      <c r="J3" s="340">
-        <f>IF(J1=$A$3,1,IF(J1&lt;$A3,K3/(1+K2/100),I3*(J2/100+1)))</f>
+      <c r="J3" s="311">
+        <f t="shared" si="0"/>
         <v>0.33725787455062667</v>
       </c>
-      <c r="K3" s="340">
-        <f>IF(K1=$A$3,1,IF(K1&lt;$A3,L3/(1+L2/100),J3*(K2/100+1)))</f>
+      <c r="K3" s="311">
+        <f t="shared" si="0"/>
         <v>0.36692416404164746</v>
       </c>
-      <c r="L3" s="340">
-        <f>IF(L1=$A$3,1,IF(L1&lt;$A3,M3/(1+M2/100),K3*(L2/100+1)))</f>
+      <c r="L3" s="311">
+        <f t="shared" si="0"/>
         <v>0.39496354076589157</v>
       </c>
-      <c r="M3" s="340">
-        <f>IF(M1=$A$3,1,IF(M1&lt;$A3,N3/(1+N2/100),L3*(M2/100+1)))</f>
+      <c r="M3" s="311">
+        <f t="shared" si="0"/>
         <v>0.44317044323682375</v>
       </c>
-      <c r="N3" s="340">
-        <f>IF(N1=$A$3,1,IF(N1&lt;$A3,O3/(1+O2/100),M3*(N2/100+1)))</f>
+      <c r="N3" s="311">
+        <f t="shared" si="0"/>
         <v>0.46884597754767043</v>
       </c>
-      <c r="O3" s="340">
-        <f>IF(O1=$A$3,1,IF(O1&lt;$A3,P3/(1+P2/100),N3*(O2/100+1)))</f>
+      <c r="O3" s="311">
+        <f t="shared" si="0"/>
         <v>0.49944808887973591</v>
       </c>
-      <c r="P3" s="340">
-        <f>IF(P1=$A$3,1,IF(P1&lt;$A3,Q3/(1+Q2/100),O3*(P2/100+1)))</f>
+      <c r="P3" s="311">
+        <f t="shared" si="0"/>
         <v>0.52666334799020664</v>
       </c>
-      <c r="Q3" s="340">
-        <f>IF(Q1=$A$3,1,IF(Q1&lt;$A3,R3/(1+R2/100),P3*(Q2/100+1)))</f>
+      <c r="Q3" s="311">
+        <f t="shared" si="0"/>
         <v>0.55970701629807973</v>
       </c>
-      <c r="R3" s="340">
-        <f>IF(R1=$A$3,1,IF(R1&lt;$A3,S3/(1+S2/100),Q3*(R2/100+1)))</f>
+      <c r="R3" s="311">
+        <f t="shared" si="0"/>
         <v>0.6092371122719199</v>
       </c>
-      <c r="S3" s="340">
-        <f>IF(S1=$A$3,1,IF(S1&lt;$A3,T3/(1+T2/100),R3*(S2/100+1)))</f>
+      <c r="S3" s="311">
+        <f t="shared" si="0"/>
         <v>0.66304230738977243</v>
       </c>
-      <c r="T3" s="340">
-        <f>IF(T1=$A$3,1,IF(T1&lt;$A3,U3/(1+U2/100),S3*(T2/100+1)))</f>
+      <c r="T3" s="311">
+        <f t="shared" si="0"/>
         <v>0.71280039257495198</v>
       </c>
-      <c r="U3" s="339">
-        <f>IF(U1=$A$3,1,IF(U1&lt;$A3,V3/(1+V2/100),T3*(U2/100+1)))</f>
+      <c r="U3" s="310">
+        <f t="shared" si="0"/>
         <v>0.7580705364703485</v>
       </c>
-      <c r="V3" s="339">
-        <f>IF(V1=$A$3,1,IF(V1&lt;$A3,W3/(1+W2/100),U3*(V2/100+1)))</f>
+      <c r="V3" s="310">
+        <f t="shared" si="0"/>
         <v>0.80849574192782814</v>
       </c>
-      <c r="W3" s="339">
-        <f>IF(W1=$A$3,1,IF(W1&lt;$A3,X3/(1+X2/100),V3*(W2/100+1)))</f>
+      <c r="W3" s="310">
+        <f t="shared" si="0"/>
         <v>0.8530618582378503</v>
       </c>
-      <c r="X3" s="357">
-        <f>IF(X1=$A$3,1,IF(X1&lt;$A3,Y3/(1+Y2/100),W3*(X2/100+1)))</f>
+      <c r="X3" s="328">
+        <f t="shared" si="0"/>
         <v>0.90412302863815563</v>
       </c>
-      <c r="Y3" s="357">
-        <f>IF(Y1=$A$3,1,IF(Y1&lt;$A3,Z3/(1+Z2/100),X3*(Y2/100+1)))</f>
+      <c r="Y3" s="328">
+        <f t="shared" si="0"/>
         <v>0.95652173913043481</v>
       </c>
-      <c r="Z3" s="357">
+      <c r="Z3" s="328">
         <f>IF(Z1=$A$3,1,IF(Z1&lt;$A3,#REF!/(1+#REF!/100),Y3*(Z2/100+1)))</f>
         <v>1</v>
       </c>
-      <c r="AA3" s="357">
+      <c r="AA3" s="328">
         <f>IF(AA1=$A$3,1,IF(AA1&lt;$A3,#REF!/(1+#REF!/100),Z3*(AA2/100+1)))</f>
         <v>1.0634057971014492</v>
       </c>
-      <c r="AB3" s="356">
+      <c r="AB3" s="327">
         <f>IF(AB1=$A$3,1,IF(AB1&lt;$A3,#REF!/(1+#REF!/100),AA3*(AB2/100+1)))</f>
         <v>1.1194746376811595</v>
       </c>
-      <c r="AC3" s="356">
+      <c r="AC3" s="327">
         <f>IF(AC1=$A$3,1,IF(AC1&lt;$A3,#REF!/(1+#REF!/100),AB3*(AC2/100+1)))</f>
         <v>1.1711956521739131</v>
       </c>
-      <c r="AD3" s="356">
+      <c r="AD3" s="327">
         <f>IF(AD1=$A$3,1,IF(AD1&lt;$A3,#REF!/(1+#REF!/100),AC3*(AD2/100+1)))</f>
         <v>1.2195652173913043</v>
       </c>
-      <c r="AE3" s="355">
+      <c r="AE3" s="326">
         <f>1/AE4</f>
         <v>1.2594458438287153</v>
       </c>
-      <c r="AF3" s="354">
+      <c r="AF3" s="325">
         <f>1/AF4</f>
         <v>1.3020833333333333</v>
       </c>
-      <c r="AG3" s="350"/>
-      <c r="AH3" s="350"/>
+      <c r="AG3" s="321"/>
+      <c r="AH3" s="321"/>
     </row>
     <row r="4" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="341" t="s">
+      <c r="A4" s="312" t="s">
         <v>810</v>
       </c>
-      <c r="B4" s="340">
-        <f>1/B3</f>
+      <c r="B4" s="311">
+        <f t="shared" ref="B4:AD4" si="1">1/B3</f>
         <v>6.2398755757903315</v>
       </c>
-      <c r="C4" s="340">
-        <f>1/C3</f>
+      <c r="C4" s="311">
+        <f t="shared" si="1"/>
         <v>5.4462886005988285</v>
       </c>
-      <c r="D4" s="340">
-        <f>1/D3</f>
+      <c r="D4" s="311">
+        <f t="shared" si="1"/>
         <v>4.8159922923538652</v>
       </c>
-      <c r="E4" s="340">
-        <f>1/E3</f>
+      <c r="E4" s="311">
+        <f t="shared" si="1"/>
         <v>4.3943937132785313</v>
       </c>
-      <c r="F4" s="340">
-        <f>1/F3</f>
+      <c r="F4" s="311">
+        <f t="shared" si="1"/>
         <v>3.9858328538286698</v>
       </c>
-      <c r="G4" s="340">
-        <f>1/G3</f>
+      <c r="G4" s="311">
+        <f t="shared" si="1"/>
         <v>3.6938090766748668</v>
       </c>
-      <c r="H4" s="340">
-        <f>1/H3</f>
+      <c r="H4" s="311">
+        <f t="shared" si="1"/>
         <v>3.4206004709706588</v>
       </c>
-      <c r="I4" s="340">
-        <f>1/I3</f>
+      <c r="I4" s="311">
+        <f t="shared" si="1"/>
         <v>3.1734714835009621</v>
       </c>
-      <c r="J4" s="340">
-        <f>1/J3</f>
+      <c r="J4" s="311">
+        <f t="shared" si="1"/>
         <v>2.9650901445442375</v>
       </c>
-      <c r="K4" s="340">
-        <f>1/K3</f>
+      <c r="K4" s="311">
+        <f t="shared" si="1"/>
         <v>2.7253588016255472</v>
       </c>
-      <c r="L4" s="340">
-        <f>1/L3</f>
+      <c r="L4" s="311">
+        <f t="shared" si="1"/>
         <v>2.5318792667820809</v>
       </c>
-      <c r="M4" s="340">
-        <f>1/M3</f>
+      <c r="M4" s="311">
+        <f t="shared" si="1"/>
         <v>2.2564681721466129</v>
       </c>
-      <c r="N4" s="340">
-        <f>1/N3</f>
+      <c r="N4" s="311">
+        <f t="shared" si="1"/>
         <v>2.1328966182680409</v>
       </c>
-      <c r="O4" s="340">
-        <f>1/O3</f>
+      <c r="O4" s="311">
+        <f t="shared" si="1"/>
         <v>2.0022100840209522</v>
       </c>
-      <c r="P4" s="340">
-        <f>1/P3</f>
+      <c r="P4" s="311">
+        <f t="shared" si="1"/>
         <v>1.8987461417546663</v>
       </c>
-      <c r="Q4" s="340">
-        <f>1/Q3</f>
+      <c r="Q4" s="311">
+        <f t="shared" si="1"/>
         <v>1.7866490340143175</v>
       </c>
-      <c r="R4" s="340">
-        <f>1/R3</f>
+      <c r="R4" s="311">
+        <f t="shared" si="1"/>
         <v>1.6413970519144465</v>
       </c>
-      <c r="S4" s="340">
-        <f>1/S3</f>
+      <c r="S4" s="311">
+        <f t="shared" si="1"/>
         <v>1.5081993846467259</v>
       </c>
-      <c r="T4" s="340">
-        <f>1/T3</f>
+      <c r="T4" s="311">
+        <f t="shared" si="1"/>
         <v>1.4029172969273422</v>
       </c>
-      <c r="U4" s="339">
-        <f>1/U3</f>
+      <c r="U4" s="310">
+        <f t="shared" si="1"/>
         <v>1.3191384599328964</v>
       </c>
-      <c r="V4" s="339">
-        <f>1/V3</f>
+      <c r="V4" s="310">
+        <f t="shared" si="1"/>
         <v>1.2368648938280578</v>
       </c>
-      <c r="W4" s="339">
-        <f>1/W3</f>
+      <c r="W4" s="310">
+        <f t="shared" si="1"/>
         <v>1.1722479329525719</v>
       </c>
-      <c r="X4" s="353">
-        <f>1/X3</f>
+      <c r="X4" s="324">
+        <f t="shared" si="1"/>
         <v>1.106044164704288</v>
       </c>
-      <c r="Y4" s="353">
-        <f>1/Y3</f>
+      <c r="Y4" s="324">
+        <f t="shared" si="1"/>
         <v>1.0454545454545454</v>
       </c>
-      <c r="Z4" s="352">
-        <f>1/Z3</f>
+      <c r="Z4" s="323">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AA4" s="352">
-        <f>1/AA3</f>
+      <c r="AA4" s="323">
+        <f t="shared" si="1"/>
         <v>0.94037478705281097</v>
       </c>
-      <c r="AB4" s="351">
-        <f>1/AB3</f>
+      <c r="AB4" s="322">
+        <f t="shared" si="1"/>
         <v>0.89327615502872393</v>
       </c>
-      <c r="AC4" s="351">
-        <f>1/AC3</f>
+      <c r="AC4" s="322">
+        <f t="shared" si="1"/>
         <v>0.85382830626450112</v>
       </c>
-      <c r="AD4" s="351">
-        <f>1/AD3</f>
+      <c r="AD4" s="322">
+        <f t="shared" si="1"/>
         <v>0.81996434937611407</v>
       </c>
-      <c r="AE4" s="350">
+      <c r="AE4" s="321">
         <v>0.79400000000000004</v>
       </c>
-      <c r="AF4" s="350">
+      <c r="AF4" s="321">
         <v>0.76800000000000002</v>
       </c>
-      <c r="AG4" s="350"/>
-      <c r="AH4" s="350"/>
+      <c r="AG4" s="321"/>
+      <c r="AH4" s="321"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="258" t="s">
         <v>822</v>
       </c>
-      <c r="U5" s="337"/>
-      <c r="V5" s="337"/>
-      <c r="W5" s="337"/>
+      <c r="U5" s="308"/>
+      <c r="V5" s="308"/>
+      <c r="W5" s="308"/>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="74" t="s">
         <v>821</v>
       </c>
-      <c r="U6" s="337"/>
-      <c r="V6" s="337"/>
-      <c r="W6" s="337"/>
+      <c r="U6" s="308"/>
+      <c r="V6" s="308"/>
+      <c r="W6" s="308"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="258" t="s">
         <v>820</v>
       </c>
-      <c r="U7" s="337"/>
-      <c r="V7" s="337"/>
-      <c r="W7" s="337"/>
+      <c r="U7" s="308"/>
+      <c r="V7" s="308"/>
+      <c r="W7" s="308"/>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="U8" s="337"/>
-      <c r="V8" s="337"/>
-      <c r="W8" s="337"/>
+      <c r="U8" s="308"/>
+      <c r="V8" s="308"/>
+      <c r="W8" s="308"/>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="258" t="s">
         <v>819</v>
       </c>
-      <c r="U9" s="337"/>
-      <c r="V9" s="337"/>
-      <c r="W9" s="337"/>
+      <c r="U9" s="308"/>
+      <c r="V9" s="308"/>
+      <c r="W9" s="308"/>
     </row>
     <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="349">
+      <c r="B10" s="320">
         <v>2010</v>
       </c>
       <c r="C10" s="258" t="s">
         <v>817</v>
       </c>
-      <c r="U10" s="337"/>
-      <c r="V10" s="337"/>
-      <c r="W10" s="337"/>
+      <c r="U10" s="308"/>
+      <c r="V10" s="308"/>
+      <c r="W10" s="308"/>
       <c r="AA10" s="258">
         <v>2005</v>
       </c>
@@ -30820,23 +30833,23 @@
       <c r="A11" s="258" t="s">
         <v>818</v>
       </c>
-      <c r="U11" s="337"/>
-      <c r="V11" s="337"/>
-      <c r="W11" s="337"/>
+      <c r="U11" s="308"/>
+      <c r="V11" s="308"/>
+      <c r="W11" s="308"/>
       <c r="AA11" s="258">
         <v>2006</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="349">
+      <c r="B12" s="320">
         <v>2015</v>
       </c>
       <c r="C12" s="258" t="s">
         <v>817</v>
       </c>
-      <c r="U12" s="337"/>
-      <c r="V12" s="337"/>
-      <c r="W12" s="337"/>
+      <c r="U12" s="308"/>
+      <c r="V12" s="308"/>
+      <c r="W12" s="308"/>
       <c r="AA12" s="258">
         <v>2007</v>
       </c>
@@ -30845,9 +30858,9 @@
       <c r="A13" s="258" t="s">
         <v>816</v>
       </c>
-      <c r="U13" s="337"/>
-      <c r="V13" s="337"/>
-      <c r="W13" s="337"/>
+      <c r="U13" s="308"/>
+      <c r="V13" s="308"/>
+      <c r="W13" s="308"/>
       <c r="X13" s="258">
         <f>PRODUCT(P17:T17)</f>
         <v>1.1326254216924159</v>
@@ -30860,13 +30873,13 @@
       <c r="A14" s="258" t="s">
         <v>815</v>
       </c>
-      <c r="B14" s="348">
+      <c r="B14" s="319">
         <f>1/B15</f>
         <v>1.3191384599328964</v>
       </c>
-      <c r="U14" s="337"/>
-      <c r="V14" s="337"/>
-      <c r="W14" s="337"/>
+      <c r="U14" s="308"/>
+      <c r="V14" s="308"/>
+      <c r="W14" s="308"/>
       <c r="AA14" s="258">
         <v>2009</v>
       </c>
@@ -30875,123 +30888,123 @@
       <c r="A15" s="258" t="s">
         <v>814</v>
       </c>
-      <c r="B15" s="347">
+      <c r="B15" s="318">
         <f>SUMIF($B$1:$U$1,B10,$B$3:$U$3)</f>
         <v>0.7580705364703485</v>
       </c>
-      <c r="U15" s="337"/>
-      <c r="V15" s="337"/>
-      <c r="W15" s="337"/>
+      <c r="U15" s="308"/>
+      <c r="V15" s="308"/>
+      <c r="W15" s="308"/>
       <c r="AA15" s="258">
         <v>2010</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="U16" s="337"/>
-      <c r="W16" s="337"/>
+      <c r="U16" s="308"/>
+      <c r="W16" s="308"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="258" t="s">
         <v>813</v>
       </c>
       <c r="P17" s="258">
-        <f>(1+P19/100)</f>
+        <f t="shared" ref="P17:U17" si="2">(1+P19/100)</f>
         <v>1.0333465966170388</v>
       </c>
       <c r="Q17" s="258">
-        <f>(1+Q19/100)</f>
+        <f t="shared" si="2"/>
         <v>1.0325252979731299</v>
       </c>
       <c r="R17" s="258">
-        <f>(1+R19/100)</f>
+        <f t="shared" si="2"/>
         <v>1.0294106674465962</v>
       </c>
       <c r="S17" s="258">
-        <f>(1+S19/100)</f>
+        <f t="shared" si="2"/>
         <v>1.0217815161638351</v>
       </c>
       <c r="T17" s="258">
-        <f>(1+T19/100)</f>
+        <f t="shared" si="2"/>
         <v>1.0092363494772816</v>
       </c>
       <c r="U17" s="258">
-        <f>(1+U19/100)</f>
+        <f t="shared" si="2"/>
         <v>1.0115232634848643</v>
       </c>
-      <c r="V17" s="337">
+      <c r="V17" s="308">
         <f>V20/U20</f>
         <v>1.0273128343245979</v>
       </c>
-      <c r="W17" s="337"/>
+      <c r="W17" s="308"/>
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="336" t="s">
+      <c r="A18" s="307" t="s">
         <v>808</v>
       </c>
-      <c r="B18" s="336">
+      <c r="B18" s="307">
         <v>1991</v>
       </c>
-      <c r="C18" s="336">
+      <c r="C18" s="307">
         <v>1992</v>
       </c>
-      <c r="D18" s="336">
+      <c r="D18" s="307">
         <v>1993</v>
       </c>
-      <c r="E18" s="336">
+      <c r="E18" s="307">
         <v>1994</v>
       </c>
-      <c r="F18" s="336">
+      <c r="F18" s="307">
         <v>1995</v>
       </c>
-      <c r="G18" s="336">
+      <c r="G18" s="307">
         <v>1996</v>
       </c>
-      <c r="H18" s="336">
+      <c r="H18" s="307">
         <v>1997</v>
       </c>
-      <c r="I18" s="336">
+      <c r="I18" s="307">
         <v>1998</v>
       </c>
-      <c r="J18" s="336">
+      <c r="J18" s="307">
         <v>1999</v>
       </c>
-      <c r="K18" s="336">
+      <c r="K18" s="307">
         <v>2000</v>
       </c>
-      <c r="L18" s="336">
+      <c r="L18" s="307">
         <v>2001</v>
       </c>
-      <c r="M18" s="336">
+      <c r="M18" s="307">
         <v>2002</v>
       </c>
-      <c r="N18" s="336">
+      <c r="N18" s="307">
         <v>2003</v>
       </c>
-      <c r="O18" s="336">
+      <c r="O18" s="307">
         <v>2004</v>
       </c>
-      <c r="P18" s="336">
+      <c r="P18" s="307">
         <v>2005</v>
       </c>
-      <c r="Q18" s="336">
+      <c r="Q18" s="307">
         <v>2006</v>
       </c>
-      <c r="R18" s="336">
+      <c r="R18" s="307">
         <v>2007</v>
       </c>
-      <c r="S18" s="336">
+      <c r="S18" s="307">
         <v>2008</v>
       </c>
-      <c r="T18" s="336">
+      <c r="T18" s="307">
         <v>2009</v>
       </c>
-      <c r="U18" s="335">
+      <c r="U18" s="306">
         <v>2010</v>
       </c>
-      <c r="V18" s="335">
+      <c r="V18" s="306">
         <v>2011</v>
       </c>
-      <c r="W18" s="335">
+      <c r="W18" s="306">
         <v>2012</v>
       </c>
       <c r="X18" s="258">
@@ -31002,786 +31015,786 @@
       </c>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="334" t="s">
+      <c r="A19" s="305" t="s">
         <v>812</v>
       </c>
-      <c r="B19" s="333">
+      <c r="B19" s="304">
         <v>3.3994252378249699</v>
       </c>
-      <c r="C19" s="333">
+      <c r="C19" s="304">
         <v>2.1054788150436798</v>
       </c>
-      <c r="D19" s="333">
+      <c r="D19" s="304">
         <v>2.1924332890308</v>
       </c>
-      <c r="E19" s="333">
+      <c r="E19" s="304">
         <v>2.0360309460728101</v>
       </c>
-      <c r="F19" s="333">
+      <c r="F19" s="304">
         <v>2.3263787079223999</v>
       </c>
-      <c r="G19" s="333">
+      <c r="G19" s="304">
         <v>1.7717629484628601</v>
       </c>
-      <c r="H19" s="333">
+      <c r="H19" s="304">
         <v>1.9273567571815799</v>
       </c>
-      <c r="I19" s="333">
+      <c r="I19" s="304">
         <v>1.4055393887866201</v>
       </c>
-      <c r="J19" s="333">
+      <c r="J19" s="304">
         <v>1.46557115641922</v>
       </c>
-      <c r="K19" s="333">
+      <c r="K19" s="304">
         <v>2.1635805504784602</v>
       </c>
-      <c r="L19" s="333">
+      <c r="L19" s="304">
         <v>2.2671398465768702</v>
       </c>
-      <c r="M19" s="333">
+      <c r="M19" s="304">
         <v>1.6245670393856999</v>
       </c>
-      <c r="N19" s="333">
+      <c r="N19" s="304">
         <v>2.1553754412521502</v>
       </c>
-      <c r="O19" s="333">
+      <c r="O19" s="304">
         <v>2.8345692622040302</v>
       </c>
-      <c r="P19" s="333">
+      <c r="P19" s="304">
         <v>3.33465966170388</v>
       </c>
-      <c r="Q19" s="333">
+      <c r="Q19" s="304">
         <v>3.2525297973129899</v>
       </c>
-      <c r="R19" s="333">
+      <c r="R19" s="304">
         <v>2.9410667446596199</v>
       </c>
-      <c r="S19" s="333">
+      <c r="S19" s="304">
         <v>2.1781516163835</v>
       </c>
-      <c r="T19" s="333">
+      <c r="T19" s="304">
         <v>0.92363494772816102</v>
       </c>
-      <c r="U19" s="343">
+      <c r="U19" s="314">
         <v>1.1523263484864299</v>
       </c>
-      <c r="V19" s="343">
+      <c r="V19" s="314">
         <v>2.7312834324597901</v>
       </c>
-      <c r="W19" s="342">
+      <c r="W19" s="313">
         <v>2.7312834324597901</v>
       </c>
-      <c r="X19" s="346">
+      <c r="X19" s="317">
         <f>W19</f>
         <v>2.7312834324597901</v>
       </c>
-      <c r="Y19" s="346">
+      <c r="Y19" s="317">
         <f>X19</f>
         <v>2.7312834324597901</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20" s="341">
+      <c r="A20" s="312">
         <v>2010</v>
       </c>
-      <c r="B20" s="340">
-        <f>IF(B18=$A$20,1,IF(B18&lt;$A20,C20/(1+C19/100),A20*(B19/100+1)))</f>
+      <c r="B20" s="311">
+        <f t="shared" ref="B20:Y20" si="3">IF(B18=$A$20,1,IF(B18&lt;$A20,C20/(1+C19/100),A20*(B19/100+1)))</f>
         <v>0.67297533398349141</v>
       </c>
-      <c r="C20" s="340">
-        <f>IF(C18=$A$20,1,IF(C18&lt;$A20,D20/(1+D19/100),B20*(C19/100+1)))</f>
+      <c r="C20" s="311">
+        <f t="shared" si="3"/>
         <v>0.68714468707098331</v>
       </c>
-      <c r="D20" s="340">
-        <f>IF(D18=$A$20,1,IF(D18&lt;$A20,E20/(1+E19/100),C20*(D19/100+1)))</f>
+      <c r="D20" s="311">
+        <f t="shared" si="3"/>
         <v>0.70220987593413409</v>
       </c>
-      <c r="E20" s="340">
-        <f>IF(E18=$A$20,1,IF(E18&lt;$A20,F20/(1+F19/100),D20*(E19/100+1)))</f>
+      <c r="E20" s="311">
+        <f t="shared" si="3"/>
         <v>0.71650708631453253</v>
       </c>
-      <c r="F20" s="340">
-        <f>IF(F18=$A$20,1,IF(F18&lt;$A20,G20/(1+G19/100),E20*(F19/100+1)))</f>
+      <c r="F20" s="311">
+        <f t="shared" si="3"/>
         <v>0.73317575461130902</v>
       </c>
-      <c r="G20" s="340">
-        <f>IF(G18=$A$20,1,IF(G18&lt;$A20,H20/(1+H19/100),F20*(G19/100+1)))</f>
+      <c r="G20" s="311">
+        <f t="shared" si="3"/>
         <v>0.74616589097862518</v>
       </c>
-      <c r="H20" s="340">
-        <f>IF(H18=$A$20,1,IF(H18&lt;$A20,I20/(1+I19/100),G20*(H19/100+1)))</f>
+      <c r="H20" s="311">
+        <f t="shared" si="3"/>
         <v>0.76054716969818592</v>
       </c>
-      <c r="I20" s="340">
-        <f>IF(I18=$A$20,1,IF(I18&lt;$A20,J20/(1+J19/100),H20*(I19/100+1)))</f>
+      <c r="I20" s="311">
+        <f t="shared" si="3"/>
         <v>0.77123695973859574</v>
       </c>
-      <c r="J20" s="340">
-        <f>IF(J18=$A$20,1,IF(J18&lt;$A20,K20/(1+K19/100),I20*(J19/100+1)))</f>
+      <c r="J20" s="311">
+        <f t="shared" si="3"/>
         <v>0.782539986168169</v>
       </c>
-      <c r="K20" s="340">
-        <f>IF(K18=$A$20,1,IF(K18&lt;$A20,L20/(1+L19/100),J20*(K19/100+1)))</f>
+      <c r="K20" s="311">
+        <f t="shared" si="3"/>
         <v>0.79947086910862031</v>
       </c>
-      <c r="L20" s="340">
-        <f>IF(L18=$A$20,1,IF(L18&lt;$A20,M20/(1+M19/100),K20*(L19/100+1)))</f>
+      <c r="L20" s="311">
+        <f t="shared" si="3"/>
         <v>0.81759599174395625</v>
       </c>
-      <c r="M20" s="340">
-        <f>IF(M18=$A$20,1,IF(M18&lt;$A20,N20/(1+N19/100),L20*(M19/100+1)))</f>
+      <c r="M20" s="311">
+        <f t="shared" si="3"/>
         <v>0.8308783867411671</v>
       </c>
-      <c r="N20" s="340">
-        <f>IF(N18=$A$20,1,IF(N18&lt;$A20,O20/(1+O19/100),M20*(N19/100+1)))</f>
+      <c r="N20" s="311">
+        <f t="shared" si="3"/>
         <v>0.84878693543565831</v>
       </c>
-      <c r="O20" s="340">
-        <f>IF(O18=$A$20,1,IF(O18&lt;$A20,P20/(1+P19/100),N20*(O19/100+1)))</f>
+      <c r="O20" s="311">
+        <f t="shared" si="3"/>
         <v>0.87284638900912104</v>
       </c>
-      <c r="P20" s="340">
-        <f>IF(P18=$A$20,1,IF(P18&lt;$A20,Q20/(1+Q19/100),O20*(P19/100+1)))</f>
+      <c r="P20" s="311">
+        <f t="shared" si="3"/>
         <v>0.90195284545204713</v>
       </c>
-      <c r="Q20" s="345">
-        <f>IF(Q18=$A$20,1,IF(Q18&lt;$A20,R20/(1+R19/100),P20*(Q19/100+1)))</f>
+      <c r="Q20" s="316">
+        <f t="shared" si="3"/>
         <v>0.93128913050808726</v>
       </c>
-      <c r="R20" s="340">
-        <f>IF(R18=$A$20,1,IF(R18&lt;$A20,S20/(1+S19/100),Q20*(R19/100+1)))</f>
+      <c r="R20" s="311">
+        <f t="shared" si="3"/>
         <v>0.9586789654220903</v>
       </c>
-      <c r="S20" s="340">
-        <f>IF(S18=$A$20,1,IF(S18&lt;$A20,T20/(1+T19/100),R20*(S19/100+1)))</f>
+      <c r="S20" s="311">
+        <f t="shared" si="3"/>
         <v>0.97956044680336019</v>
       </c>
-      <c r="T20" s="340">
-        <f>IF(T18=$A$20,1,IF(T18&lt;$A20,U20/(1+U19/100),S20*(T19/100+1)))</f>
+      <c r="T20" s="311">
+        <f t="shared" si="3"/>
         <v>0.98860800942415816</v>
       </c>
-      <c r="U20" s="339">
-        <f>IF(U18=$A$20,1,IF(U18&lt;$A20,V20/(1+V19/100),T20*(U19/100+1)))</f>
+      <c r="U20" s="310">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="V20" s="339">
-        <f>IF(V18=$A$20,1,IF(V18&lt;$A20,W20/(1+W19/100),U20*(V19/100+1)))</f>
+      <c r="V20" s="310">
+        <f t="shared" si="3"/>
         <v>1.0273128343245979</v>
       </c>
-      <c r="W20" s="339">
-        <f>IF(W18=$A$20,1,IF(W18&lt;$A20,X20/(1+X19/100),V20*(W19/100+1)))</f>
+      <c r="W20" s="310">
+        <f t="shared" si="3"/>
         <v>1.0553716595680387</v>
       </c>
-      <c r="X20" s="344">
-        <f>IF(X18=$A$20,1,IF(X18&lt;$A20,Y20/(1+Y19/100),W20*(X19/100+1)))</f>
+      <c r="X20" s="315">
+        <f t="shared" si="3"/>
         <v>1.0841968508566964</v>
       </c>
-      <c r="Y20" s="344">
-        <f>IF(Y18=$A$20,1,IF(Y18&lt;$A20,Z20/(1+Z19/100),X20*(Y19/100+1)))</f>
+      <c r="Y20" s="315">
+        <f t="shared" si="3"/>
         <v>1.113809339819396</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A21" s="341" t="s">
+      <c r="A21" s="312" t="s">
         <v>810</v>
       </c>
-      <c r="B21" s="340">
-        <f>1/B20</f>
+      <c r="B21" s="311">
+        <f t="shared" ref="B21:Y21" si="4">1/B20</f>
         <v>1.4859385619392267</v>
       </c>
-      <c r="C21" s="340">
-        <f>1/C20</f>
+      <c r="C21" s="311">
+        <f t="shared" si="4"/>
         <v>1.4552975797027419</v>
       </c>
-      <c r="D21" s="340">
-        <f>1/D20</f>
+      <c r="D21" s="311">
+        <f t="shared" si="4"/>
         <v>1.424075670638671</v>
       </c>
-      <c r="E21" s="340">
-        <f>1/E20</f>
+      <c r="E21" s="311">
+        <f t="shared" si="4"/>
         <v>1.395659609095645</v>
       </c>
-      <c r="F21" s="340">
-        <f>1/F20</f>
+      <c r="F21" s="311">
+        <f t="shared" si="4"/>
         <v>1.3639294448984434</v>
       </c>
-      <c r="G21" s="340">
-        <f>1/G20</f>
+      <c r="G21" s="311">
+        <f t="shared" si="4"/>
         <v>1.3401845515726558</v>
       </c>
-      <c r="H21" s="340">
-        <f>1/H20</f>
+      <c r="H21" s="311">
+        <f t="shared" si="4"/>
         <v>1.314842839263787</v>
       </c>
-      <c r="I21" s="340">
-        <f>1/I20</f>
+      <c r="I21" s="311">
+        <f t="shared" si="4"/>
         <v>1.2966183575265138</v>
       </c>
-      <c r="J21" s="340">
-        <f>1/J20</f>
+      <c r="J21" s="311">
+        <f t="shared" si="4"/>
         <v>1.2778899707050861</v>
       </c>
-      <c r="K21" s="340">
-        <f>1/K20</f>
+      <c r="K21" s="311">
+        <f t="shared" si="4"/>
         <v>1.2508273142146655</v>
       </c>
-      <c r="L21" s="340">
-        <f>1/L20</f>
+      <c r="L21" s="311">
+        <f t="shared" si="4"/>
         <v>1.2230979727126239</v>
       </c>
-      <c r="M21" s="340">
-        <f>1/M20</f>
+      <c r="M21" s="311">
+        <f t="shared" si="4"/>
         <v>1.2035455681091356</v>
       </c>
-      <c r="N21" s="340">
-        <f>1/N20</f>
+      <c r="N21" s="311">
+        <f t="shared" si="4"/>
         <v>1.1781519698895087</v>
       </c>
-      <c r="O21" s="340">
-        <f>1/O20</f>
+      <c r="O21" s="311">
+        <f t="shared" si="4"/>
         <v>1.1456769628562331</v>
       </c>
-      <c r="P21" s="340">
-        <f>1/P20</f>
+      <c r="P21" s="311">
+        <f t="shared" si="4"/>
         <v>1.1087054107566043</v>
       </c>
-      <c r="Q21" s="340">
-        <f>1/Q20</f>
+      <c r="Q21" s="311">
+        <f t="shared" si="4"/>
         <v>1.0737803838153097</v>
       </c>
-      <c r="R21" s="340">
-        <f>1/R20</f>
+      <c r="R21" s="311">
+        <f t="shared" si="4"/>
         <v>1.0431020561296207</v>
       </c>
-      <c r="S21" s="340">
-        <f>1/S20</f>
+      <c r="S21" s="311">
+        <f t="shared" si="4"/>
         <v>1.020866045850811</v>
       </c>
-      <c r="T21" s="340">
-        <f>1/T20</f>
+      <c r="T21" s="311">
+        <f t="shared" si="4"/>
         <v>1.0115232634848643</v>
       </c>
-      <c r="U21" s="339">
-        <f>1/U20</f>
+      <c r="U21" s="310">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="V21" s="339">
-        <f>1/V20</f>
+      <c r="V21" s="310">
+        <f t="shared" si="4"/>
         <v>0.97341332317477125</v>
       </c>
-      <c r="W21" s="339">
-        <f>1/W20</f>
+      <c r="W21" s="310">
+        <f t="shared" si="4"/>
         <v>0.94753349773415163</v>
       </c>
-      <c r="X21" s="339">
-        <f>1/X20</f>
+      <c r="X21" s="310">
+        <f t="shared" si="4"/>
         <v>0.9223417308488151</v>
       </c>
-      <c r="Y21" s="339">
-        <f>1/Y20</f>
+      <c r="Y21" s="310">
+        <f t="shared" si="4"/>
         <v>0.89781972932831555</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="U22" s="337"/>
-      <c r="V22" s="337"/>
-      <c r="W22" s="337"/>
+      <c r="U22" s="308"/>
+      <c r="V22" s="308"/>
+      <c r="W22" s="308"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A23" s="338" t="s">
+      <c r="A23" s="309" t="s">
         <v>811</v>
       </c>
-      <c r="U23" s="337"/>
-      <c r="V23" s="337"/>
-      <c r="W23" s="337"/>
+      <c r="U23" s="308"/>
+      <c r="V23" s="308"/>
+      <c r="W23" s="308"/>
     </row>
     <row r="24" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="336" t="s">
+      <c r="A24" s="307" t="s">
         <v>808</v>
       </c>
-      <c r="B24" s="336">
+      <c r="B24" s="307">
         <v>1991</v>
       </c>
-      <c r="C24" s="336">
+      <c r="C24" s="307">
         <v>1992</v>
       </c>
-      <c r="D24" s="336">
+      <c r="D24" s="307">
         <v>1993</v>
       </c>
-      <c r="E24" s="336">
+      <c r="E24" s="307">
         <v>1994</v>
       </c>
-      <c r="F24" s="336">
+      <c r="F24" s="307">
         <v>1995</v>
       </c>
-      <c r="G24" s="336">
+      <c r="G24" s="307">
         <v>1996</v>
       </c>
-      <c r="H24" s="336">
+      <c r="H24" s="307">
         <v>1997</v>
       </c>
-      <c r="I24" s="336">
+      <c r="I24" s="307">
         <v>1998</v>
       </c>
-      <c r="J24" s="336">
+      <c r="J24" s="307">
         <v>1999</v>
       </c>
-      <c r="K24" s="336">
+      <c r="K24" s="307">
         <v>2000</v>
       </c>
-      <c r="L24" s="336">
+      <c r="L24" s="307">
         <v>2001</v>
       </c>
-      <c r="M24" s="336">
+      <c r="M24" s="307">
         <v>2002</v>
       </c>
-      <c r="N24" s="336">
+      <c r="N24" s="307">
         <v>2003</v>
       </c>
-      <c r="O24" s="336">
+      <c r="O24" s="307">
         <v>2004</v>
       </c>
-      <c r="P24" s="336">
+      <c r="P24" s="307">
         <v>2005</v>
       </c>
-      <c r="Q24" s="336">
+      <c r="Q24" s="307">
         <v>2006</v>
       </c>
-      <c r="R24" s="336">
+      <c r="R24" s="307">
         <v>2007</v>
       </c>
-      <c r="S24" s="336">
+      <c r="S24" s="307">
         <v>2008</v>
       </c>
-      <c r="T24" s="336">
+      <c r="T24" s="307">
         <v>2009</v>
       </c>
-      <c r="U24" s="335">
+      <c r="U24" s="306">
         <v>2010</v>
       </c>
-      <c r="V24" s="335">
+      <c r="V24" s="306">
         <v>2011</v>
       </c>
-      <c r="W24" s="335">
+      <c r="W24" s="306">
         <v>2012</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="334" t="s">
+      <c r="A25" s="305" t="s">
         <v>785</v>
       </c>
-      <c r="B25" s="333">
+      <c r="B25" s="304">
         <v>2.7613150000000002</v>
       </c>
-      <c r="C25" s="333">
+      <c r="C25" s="304">
         <v>2.8520141666666698</v>
       </c>
-      <c r="D25" s="333">
+      <c r="D25" s="304">
         <v>3.2677415833333301</v>
       </c>
-      <c r="E25" s="333">
+      <c r="E25" s="304">
         <v>3.5507983333333302</v>
       </c>
-      <c r="F25" s="333">
+      <c r="F25" s="304">
         <v>3.6270850000000001</v>
       </c>
-      <c r="G25" s="333">
+      <c r="G25" s="304">
         <v>4.2993491666666701</v>
       </c>
-      <c r="H25" s="333">
+      <c r="H25" s="304">
         <v>4.6079616666666698</v>
       </c>
-      <c r="I25" s="333">
+      <c r="I25" s="304">
         <v>5.52828416666667</v>
       </c>
-      <c r="J25" s="333">
+      <c r="J25" s="304">
         <v>6.1094841666666699</v>
       </c>
-      <c r="K25" s="333">
+      <c r="K25" s="304">
         <v>6.9398283333333302</v>
       </c>
-      <c r="L25" s="333">
+      <c r="L25" s="304">
         <v>8.6091808333333297</v>
       </c>
-      <c r="M25" s="333">
+      <c r="M25" s="304">
         <v>10.540746666666699</v>
       </c>
-      <c r="N25" s="333">
+      <c r="N25" s="304">
         <v>7.5647491666666697</v>
       </c>
-      <c r="O25" s="333">
+      <c r="O25" s="304">
         <v>6.4596925000000001</v>
       </c>
-      <c r="P25" s="333">
+      <c r="P25" s="304">
         <v>6.3593283333333304</v>
       </c>
-      <c r="Q25" s="333">
+      <c r="Q25" s="304">
         <v>6.7715491666666701</v>
       </c>
-      <c r="R25" s="333">
+      <c r="R25" s="304">
         <v>7.0453650000000003</v>
       </c>
-      <c r="S25" s="333">
+      <c r="S25" s="304">
         <v>8.26122333333333</v>
       </c>
-      <c r="T25" s="333">
+      <c r="T25" s="304">
         <v>8.4736741582488797</v>
       </c>
-      <c r="U25" s="332">
+      <c r="U25" s="303">
         <v>7.3212219611528804</v>
       </c>
-      <c r="V25" s="343">
+      <c r="V25" s="314">
         <v>7.2611321323273499</v>
       </c>
-      <c r="W25" s="342">
+      <c r="W25" s="313">
         <v>8.5</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A26" s="341">
+      <c r="A26" s="312">
         <v>2005</v>
       </c>
-      <c r="B26" s="340">
-        <f>IF(B24=$A$26,1,IF(B24&lt;$A26,C26/(1+C25/100),A26*(B25/100+1)))</f>
+      <c r="B26" s="311">
+        <f t="shared" ref="B26:W26" si="5">IF(B24=$A$26,1,IF(B24&lt;$A26,C26/(1+C25/100),A26*(B25/100+1)))</f>
         <v>0.45926906270745477</v>
       </c>
-      <c r="C26" s="340">
-        <f>IF(C24=$A$26,1,IF(C24&lt;$A26,D26/(1+D25/100),B26*(C25/100+1)))</f>
+      <c r="C26" s="311">
+        <f t="shared" si="5"/>
         <v>0.4723674814389886</v>
       </c>
-      <c r="D26" s="340">
-        <f>IF(D24=$A$26,1,IF(D24&lt;$A26,E26/(1+E25/100),C26*(D25/100+1)))</f>
+      <c r="D26" s="311">
+        <f t="shared" si="5"/>
         <v>0.48780323005611481</v>
       </c>
-      <c r="E26" s="340">
-        <f>IF(E24=$A$26,1,IF(E24&lt;$A26,F26/(1+F25/100),D26*(E25/100+1)))</f>
+      <c r="E26" s="311">
+        <f t="shared" si="5"/>
         <v>0.50512413901889353</v>
       </c>
-      <c r="F26" s="340">
-        <f>IF(F24=$A$26,1,IF(F24&lt;$A26,G26/(1+G25/100),E26*(F25/100+1)))</f>
+      <c r="F26" s="311">
+        <f t="shared" si="5"/>
         <v>0.52344542089662693</v>
       </c>
-      <c r="G26" s="340">
-        <f>IF(G24=$A$26,1,IF(G24&lt;$A26,H26/(1+H25/100),F26*(G25/100+1)))</f>
+      <c r="G26" s="311">
+        <f t="shared" si="5"/>
         <v>0.54595016723790091</v>
       </c>
-      <c r="H26" s="340">
-        <f>IF(H24=$A$26,1,IF(H24&lt;$A26,I26/(1+I25/100),G26*(H25/100+1)))</f>
+      <c r="H26" s="311">
+        <f t="shared" si="5"/>
         <v>0.57110734166332588</v>
       </c>
-      <c r="I26" s="340">
-        <f>IF(I24=$A$26,1,IF(I24&lt;$A26,J26/(1+J25/100),H26*(I25/100+1)))</f>
+      <c r="I26" s="311">
+        <f t="shared" si="5"/>
         <v>0.60267977840717046</v>
       </c>
-      <c r="J26" s="340">
-        <f>IF(J24=$A$26,1,IF(J24&lt;$A26,K26/(1+K25/100),I26*(J25/100+1)))</f>
+      <c r="J26" s="311">
+        <f t="shared" si="5"/>
         <v>0.63950040404465835</v>
       </c>
-      <c r="K26" s="340">
-        <f>IF(K24=$A$26,1,IF(K24&lt;$A26,L26/(1+L25/100),J26*(K25/100+1)))</f>
+      <c r="K26" s="311">
+        <f t="shared" si="5"/>
         <v>0.68388063427633072</v>
       </c>
-      <c r="L26" s="340">
-        <f>IF(L24=$A$26,1,IF(L24&lt;$A26,M26/(1+M25/100),K26*(L25/100+1)))</f>
+      <c r="L26" s="311">
+        <f t="shared" si="5"/>
         <v>0.742757154765327</v>
       </c>
-      <c r="M26" s="340">
-        <f>IF(M24=$A$26,1,IF(M24&lt;$A26,N26/(1+N25/100),L26*(M25/100+1)))</f>
+      <c r="M26" s="311">
+        <f t="shared" si="5"/>
         <v>0.82104930479768157</v>
       </c>
-      <c r="N26" s="340">
-        <f>IF(N24=$A$26,1,IF(N24&lt;$A26,O26/(1+O25/100),M26*(N25/100+1)))</f>
+      <c r="N26" s="311">
+        <f t="shared" si="5"/>
         <v>0.88315962524028668</v>
       </c>
-      <c r="O26" s="340">
-        <f>IF(O24=$A$26,1,IF(O24&lt;$A26,P26/(1+P25/100),N26*(O25/100+1)))</f>
+      <c r="O26" s="311">
+        <f t="shared" si="5"/>
         <v>0.94020902131496165</v>
       </c>
-      <c r="P26" s="340">
-        <f>IF(P24=$A$26,1,IF(P24&lt;$A26,Q26/(1+Q25/100),O26*(P25/100+1)))</f>
+      <c r="P26" s="311">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="Q26" s="340">
-        <f>IF(Q24=$A$26,1,IF(Q24&lt;$A26,R26/(1+R25/100),P26*(Q25/100+1)))</f>
+      <c r="Q26" s="311">
+        <f t="shared" si="5"/>
         <v>1.0677154916666667</v>
       </c>
-      <c r="R26" s="340">
-        <f>IF(R24=$A$26,1,IF(R24&lt;$A26,S26/(1+S25/100),Q26*(R25/100+1)))</f>
+      <c r="R26" s="311">
+        <f t="shared" si="5"/>
         <v>1.142939945216128</v>
       </c>
-      <c r="S26" s="340">
-        <f>IF(S24=$A$26,1,IF(S24&lt;$A26,T26/(1+T25/100),R26*(S25/100+1)))</f>
+      <c r="S26" s="311">
+        <f t="shared" si="5"/>
         <v>1.2373607666563098</v>
       </c>
-      <c r="T26" s="340">
-        <f>IF(T24=$A$26,1,IF(T24&lt;$A26,U26/(1+U25/100),S26*(T25/100+1)))</f>
+      <c r="T26" s="311">
+        <f t="shared" si="5"/>
         <v>1.3422106861847758</v>
       </c>
-      <c r="U26" s="339">
-        <f>IF(U24=$A$26,1,IF(U24&lt;$A26,V26/(1+V25/100),T26*(U25/100+1)))</f>
+      <c r="U26" s="310">
+        <f t="shared" si="5"/>
         <v>1.4404769097066763</v>
       </c>
-      <c r="V26" s="339">
-        <f>IF(V24=$A$26,1,IF(V24&lt;$A26,W26/(1+W25/100),U26*(V25/100+1)))</f>
+      <c r="V26" s="310">
+        <f t="shared" si="5"/>
         <v>1.5450718414561437</v>
       </c>
-      <c r="W26" s="339">
-        <f>IF(W24=$A$26,1,IF(W24&lt;$A26,X26/(1+X25/100),V26*(W25/100+1)))</f>
+      <c r="W26" s="310">
+        <f t="shared" si="5"/>
         <v>1.6764029479799158</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A27" s="341" t="s">
+      <c r="A27" s="312" t="s">
         <v>810</v>
       </c>
-      <c r="B27" s="340">
-        <f>1/B26</f>
+      <c r="B27" s="311">
+        <f t="shared" ref="B27:W27" si="6">1/B26</f>
         <v>2.1773728761629654</v>
       </c>
-      <c r="C27" s="340">
-        <f>1/C26</f>
+      <c r="C27" s="311">
+        <f t="shared" si="6"/>
         <v>2.1169958544852983</v>
       </c>
-      <c r="D27" s="340">
-        <f>1/D26</f>
+      <c r="D27" s="311">
+        <f t="shared" si="6"/>
         <v>2.0500069257125753</v>
       </c>
-      <c r="E27" s="340">
-        <f>1/E26</f>
+      <c r="E27" s="311">
+        <f t="shared" si="6"/>
         <v>1.9797113674715836</v>
       </c>
-      <c r="F27" s="340">
-        <f>1/F26</f>
+      <c r="F27" s="311">
+        <f t="shared" si="6"/>
         <v>1.9104188518586465</v>
       </c>
-      <c r="G27" s="340">
-        <f>1/G26</f>
+      <c r="G27" s="311">
+        <f t="shared" si="6"/>
         <v>1.8316690057249205</v>
       </c>
-      <c r="H27" s="340">
-        <f>1/H26</f>
+      <c r="H27" s="311">
+        <f t="shared" si="6"/>
         <v>1.7509843194933241</v>
       </c>
-      <c r="I27" s="340">
-        <f>1/I26</f>
+      <c r="I27" s="311">
+        <f t="shared" si="6"/>
         <v>1.6592559362832977</v>
       </c>
-      <c r="J27" s="340">
-        <f>1/J26</f>
+      <c r="J27" s="311">
+        <f t="shared" si="6"/>
         <v>1.563720669565311</v>
       </c>
-      <c r="K27" s="340">
-        <f>1/K26</f>
+      <c r="K27" s="311">
+        <f t="shared" si="6"/>
         <v>1.4622434820927204</v>
       </c>
-      <c r="L27" s="340">
-        <f>1/L26</f>
+      <c r="L27" s="311">
+        <f t="shared" si="6"/>
         <v>1.3463350619839516</v>
       </c>
-      <c r="M27" s="340">
-        <f>1/M26</f>
+      <c r="M27" s="311">
+        <f t="shared" si="6"/>
         <v>1.2179536529129813</v>
       </c>
-      <c r="N27" s="340">
-        <f>1/N26</f>
+      <c r="N27" s="311">
+        <f t="shared" si="6"/>
         <v>1.1322981388873203</v>
       </c>
-      <c r="O27" s="340">
-        <f>1/O26</f>
+      <c r="O27" s="311">
+        <f t="shared" si="6"/>
         <v>1.0635932833333333</v>
       </c>
-      <c r="P27" s="340">
-        <f>1/P26</f>
+      <c r="P27" s="311">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="Q27" s="340">
-        <f>1/Q26</f>
+      <c r="Q27" s="311">
+        <f t="shared" si="6"/>
         <v>0.93657908666196721</v>
       </c>
-      <c r="R27" s="340">
-        <f>1/R26</f>
+      <c r="R27" s="311">
+        <f t="shared" si="6"/>
         <v>0.87493660903670811</v>
       </c>
-      <c r="S27" s="340">
-        <f>1/S26</f>
+      <c r="S27" s="311">
+        <f t="shared" si="6"/>
         <v>0.80817173693188604</v>
       </c>
-      <c r="T27" s="340">
-        <f>1/T26</f>
+      <c r="T27" s="311">
+        <f t="shared" si="6"/>
         <v>0.74503951599617557</v>
       </c>
-      <c r="U27" s="339">
-        <f>1/U26</f>
+      <c r="U27" s="310">
+        <f t="shared" si="6"/>
         <v>0.69421452941139439</v>
       </c>
-      <c r="V27" s="339">
-        <f>1/V26</f>
+      <c r="V27" s="310">
+        <f t="shared" si="6"/>
         <v>0.64721909568784575</v>
       </c>
-      <c r="W27" s="339">
-        <f>1/W26</f>
+      <c r="W27" s="310">
+        <f t="shared" si="6"/>
         <v>0.59651529556483485</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="U28" s="337"/>
-      <c r="V28" s="337"/>
-      <c r="W28" s="337"/>
+      <c r="U28" s="308"/>
+      <c r="V28" s="308"/>
+      <c r="W28" s="308"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A29" s="338" t="s">
+      <c r="A29" s="309" t="s">
         <v>809</v>
       </c>
-      <c r="U29" s="337"/>
-      <c r="V29" s="337"/>
-      <c r="W29" s="337"/>
+      <c r="U29" s="308"/>
+      <c r="V29" s="308"/>
+      <c r="W29" s="308"/>
     </row>
     <row r="30" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="336" t="s">
+      <c r="A30" s="307" t="s">
         <v>808</v>
       </c>
-      <c r="B30" s="336">
+      <c r="B30" s="307">
         <v>1991</v>
       </c>
-      <c r="C30" s="336">
+      <c r="C30" s="307">
         <v>1992</v>
       </c>
-      <c r="D30" s="336">
+      <c r="D30" s="307">
         <v>1993</v>
       </c>
-      <c r="E30" s="336">
+      <c r="E30" s="307">
         <v>1994</v>
       </c>
-      <c r="F30" s="336">
+      <c r="F30" s="307">
         <v>1995</v>
       </c>
-      <c r="G30" s="336">
+      <c r="G30" s="307">
         <v>1996</v>
       </c>
-      <c r="H30" s="336">
+      <c r="H30" s="307">
         <v>1997</v>
       </c>
-      <c r="I30" s="336">
+      <c r="I30" s="307">
         <v>1998</v>
       </c>
-      <c r="J30" s="336">
+      <c r="J30" s="307">
         <v>1999</v>
       </c>
-      <c r="K30" s="336">
+      <c r="K30" s="307">
         <v>2000</v>
       </c>
-      <c r="L30" s="336">
+      <c r="L30" s="307">
         <v>2001</v>
       </c>
-      <c r="M30" s="336">
+      <c r="M30" s="307">
         <v>2002</v>
       </c>
-      <c r="N30" s="336">
+      <c r="N30" s="307">
         <v>2003</v>
       </c>
-      <c r="O30" s="336">
+      <c r="O30" s="307">
         <v>2004</v>
       </c>
-      <c r="P30" s="336">
+      <c r="P30" s="307">
         <v>2005</v>
       </c>
-      <c r="Q30" s="336">
+      <c r="Q30" s="307">
         <v>2006</v>
       </c>
-      <c r="R30" s="336">
+      <c r="R30" s="307">
         <v>2007</v>
       </c>
-      <c r="S30" s="336">
+      <c r="S30" s="307">
         <v>2008</v>
       </c>
-      <c r="T30" s="336">
+      <c r="T30" s="307">
         <v>2009</v>
       </c>
-      <c r="U30" s="335">
+      <c r="U30" s="306">
         <v>2010</v>
       </c>
-      <c r="V30" s="335">
+      <c r="V30" s="306">
         <v>2011</v>
       </c>
-      <c r="W30" s="335">
+      <c r="W30" s="306">
         <v>2012</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="334" t="s">
+      <c r="A31" s="305" t="s">
         <v>785</v>
       </c>
-      <c r="B31" s="333">
+      <c r="B31" s="304">
         <v>120.919166666666</v>
       </c>
-      <c r="C31" s="333">
+      <c r="C31" s="304">
         <v>124.9175</v>
       </c>
-      <c r="D31" s="333">
+      <c r="D31" s="304">
         <v>122.595</v>
       </c>
-      <c r="E31" s="333">
+      <c r="E31" s="304">
         <v>117.354166666667</v>
       </c>
-      <c r="F31" s="333">
+      <c r="F31" s="304">
         <v>114.07250000000001</v>
       </c>
-      <c r="G31" s="333">
+      <c r="G31" s="304">
         <v>105.07</v>
       </c>
-      <c r="H31" s="333">
+      <c r="H31" s="304">
         <v>110.886666666667</v>
       </c>
-      <c r="I31" s="333">
+      <c r="I31" s="304">
         <v>101.948333333333</v>
       </c>
-      <c r="J31" s="333">
+      <c r="J31" s="304">
         <v>96.432500000000005</v>
       </c>
-      <c r="K31" s="333">
+      <c r="K31" s="304">
         <v>93.360833333333304</v>
       </c>
-      <c r="L31" s="333">
+      <c r="L31" s="304">
         <v>82.358333333333306</v>
       </c>
-      <c r="M31" s="333">
+      <c r="M31" s="304">
         <v>70.561666666666696</v>
       </c>
-      <c r="N31" s="333">
+      <c r="N31" s="304">
         <v>91.406666666666695</v>
       </c>
-      <c r="O31" s="333">
+      <c r="O31" s="304">
         <v>99.689166666666793</v>
       </c>
-      <c r="P31" s="333">
+      <c r="P31" s="304">
         <v>100</v>
       </c>
-      <c r="Q31" s="333">
+      <c r="Q31" s="304">
         <v>96.115833333333299</v>
       </c>
-      <c r="R31" s="333">
+      <c r="R31" s="304">
         <v>90.378333333333302</v>
       </c>
-      <c r="S31" s="333">
+      <c r="S31" s="304">
         <v>80.405000000000001</v>
       </c>
-      <c r="T31" s="333">
+      <c r="T31" s="304">
         <v>87.792500000000004</v>
       </c>
-      <c r="U31" s="332">
+      <c r="U31" s="303">
         <v>101.2</v>
       </c>
-      <c r="V31" s="332">
+      <c r="V31" s="303">
         <v>99.1</v>
       </c>
-      <c r="W31" s="332"/>
+      <c r="W31" s="303"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="258" t="s">
         <v>807</v>
       </c>
-      <c r="F33" s="331">
+      <c r="F33" s="302">
         <f>[3]PRI!E51</f>
         <v>11.914999999999999</v>
       </c>
@@ -31813,50 +31826,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="367" t="s">
+      <c r="B1" s="338" t="s">
         <v>833</v>
       </c>
-      <c r="C1" s="367"/>
-      <c r="D1" s="367"/>
-      <c r="E1" s="367"/>
-      <c r="F1" s="368"/>
-      <c r="G1" s="368"/>
+      <c r="C1" s="338"/>
+      <c r="D1" s="338"/>
+      <c r="E1" s="338"/>
+      <c r="F1" s="339"/>
+      <c r="G1" s="339"/>
     </row>
     <row r="2" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="368"/>
-      <c r="C2" s="368"/>
-      <c r="D2" s="368"/>
-      <c r="E2" s="368"/>
-      <c r="F2" s="368"/>
-      <c r="G2" s="368"/>
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="339"/>
+      <c r="G2" s="339"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="369" t="s">
+      <c r="B3" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="370"/>
-      <c r="D3" s="370"/>
-      <c r="E3" s="370"/>
-      <c r="F3" s="370"/>
-      <c r="G3" s="370"/>
+      <c r="C3" s="341"/>
+      <c r="D3" s="341"/>
+      <c r="E3" s="341"/>
+      <c r="F3" s="341"/>
+      <c r="G3" s="341"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="371" t="s">
+      <c r="B4" s="342" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="371" t="s">
+      <c r="C4" s="342" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="371" t="s">
+      <c r="D4" s="342" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="371" t="s">
+      <c r="E4" s="342" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="371" t="s">
+      <c r="F4" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="371" t="s">
+      <c r="G4" s="342" t="s">
         <v>20</v>
       </c>
     </row>
@@ -31992,8 +32005,8 @@
   </sheetPr>
   <dimension ref="A1:AE24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32140,7 +32153,7 @@
         <v>806</v>
       </c>
       <c r="X3" s="284" t="s">
-        <v>806</v>
+        <v>837</v>
       </c>
       <c r="Y3" s="258" t="s">
         <v>161</v>
@@ -32309,7 +32322,7 @@
       </c>
       <c r="M6" s="270"/>
       <c r="N6" s="268">
-        <v>2028</v>
+        <v>2080</v>
       </c>
       <c r="O6" s="262">
         <f>$O$1*'Hydrogen-Other'!R30</f>
@@ -32490,7 +32503,7 @@
       </c>
       <c r="M10" s="261"/>
       <c r="N10" s="268">
-        <v>2028</v>
+        <v>2080</v>
       </c>
       <c r="O10" s="262">
         <f>O6</f>
@@ -33974,7 +33987,7 @@
   </sheetPr>
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CAPACT-> CAPUNIT in H2 production
</commit_message>
<xml_diff>
--- a/SubRes_TMPL/SubRES_SUP_Hydrogen.xlsx
+++ b/SubRes_TMPL/SubRES_SUP_Hydrogen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SubRes_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A88EE2-E522-4B2B-BE35-6C8DAFD1972F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AE360E-D1EE-4953-870D-D968BC3D8617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="26610" windowHeight="13740" activeTab="2" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="26610" windowHeight="13740" activeTab="2" xr2:uid="{62F67F8D-DFD4-4ADE-8356-63F780461C4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="7" r:id="rId1"/>
@@ -1184,7 +1184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="839">
   <si>
     <t>Document type:</t>
   </si>
@@ -5448,6 +5448,9 @@
   </si>
   <si>
     <t>ENV_ACT~CH4C</t>
+  </si>
+  <si>
+    <t>CAPUNIT</t>
   </si>
 </sst>
 </file>
@@ -7416,35 +7419,35 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -7467,28 +7470,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -20636,16 +20639,16 @@
       <c r="K6" s="204" t="s">
         <v>546</v>
       </c>
-      <c r="L6" s="346" t="s">
+      <c r="L6" s="363" t="s">
         <v>545</v>
       </c>
-      <c r="M6" s="347"/>
-      <c r="N6" s="348"/>
-      <c r="O6" s="346" t="s">
+      <c r="M6" s="364"/>
+      <c r="N6" s="365"/>
+      <c r="O6" s="363" t="s">
         <v>484</v>
       </c>
-      <c r="P6" s="347"/>
-      <c r="Q6" s="348"/>
+      <c r="P6" s="364"/>
+      <c r="Q6" s="365"/>
       <c r="X6" s="144" t="s">
         <v>544</v>
       </c>
@@ -20657,9 +20660,9 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
-      <c r="I7" s="354"/>
-      <c r="J7" s="354"/>
-      <c r="K7" s="354"/>
+      <c r="I7" s="370"/>
+      <c r="J7" s="370"/>
+      <c r="K7" s="370"/>
       <c r="L7" s="203">
         <v>2000</v>
       </c>
@@ -20737,15 +20740,15 @@
       </c>
     </row>
     <row r="9" spans="1:28" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="355" t="s">
+      <c r="A9" s="349" t="s">
         <v>536</v>
       </c>
-      <c r="B9" s="355"/>
-      <c r="C9" s="355"/>
-      <c r="D9" s="355"/>
-      <c r="E9" s="355"/>
-      <c r="F9" s="355"/>
-      <c r="G9" s="355"/>
+      <c r="B9" s="349"/>
+      <c r="C9" s="349"/>
+      <c r="D9" s="349"/>
+      <c r="E9" s="349"/>
+      <c r="F9" s="349"/>
+      <c r="G9" s="349"/>
       <c r="I9" s="200" t="s">
         <v>409</v>
       </c>
@@ -21321,25 +21324,25 @@
       <c r="K26" s="150" t="s">
         <v>486</v>
       </c>
-      <c r="L26" s="353" t="s">
+      <c r="L26" s="350" t="s">
         <v>485</v>
       </c>
-      <c r="M26" s="353"/>
-      <c r="N26" s="353"/>
-      <c r="O26" s="353" t="s">
+      <c r="M26" s="350"/>
+      <c r="N26" s="350"/>
+      <c r="O26" s="350" t="s">
         <v>484</v>
       </c>
-      <c r="P26" s="353"/>
-      <c r="Q26" s="353"/>
-      <c r="R26" s="353" t="s">
+      <c r="P26" s="350"/>
+      <c r="Q26" s="350"/>
+      <c r="R26" s="350" t="s">
         <v>483</v>
       </c>
-      <c r="S26" s="353"/>
-      <c r="T26" s="353"/>
-      <c r="U26" s="363" t="s">
+      <c r="S26" s="350"/>
+      <c r="T26" s="350"/>
+      <c r="U26" s="353" t="s">
         <v>414</v>
       </c>
-      <c r="V26" s="363"/>
+      <c r="V26" s="353"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
@@ -22391,13 +22394,13 @@
       <c r="N45" s="134"/>
     </row>
     <row r="46" spans="1:35" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I46" s="349" t="s">
+      <c r="I46" s="366" t="s">
         <v>419</v>
       </c>
-      <c r="J46" s="349" t="s">
+      <c r="J46" s="366" t="s">
         <v>418</v>
       </c>
-      <c r="K46" s="351" t="s">
+      <c r="K46" s="368" t="s">
         <v>417</v>
       </c>
       <c r="L46" s="356" t="s">
@@ -22413,9 +22416,9 @@
       <c r="A47" s="159" t="s">
         <v>446</v>
       </c>
-      <c r="I47" s="350"/>
-      <c r="J47" s="350"/>
-      <c r="K47" s="352"/>
+      <c r="I47" s="367"/>
+      <c r="J47" s="367"/>
+      <c r="K47" s="369"/>
       <c r="L47" s="149">
         <v>2000</v>
       </c>
@@ -22450,15 +22453,15 @@
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="355" t="s">
+      <c r="A49" s="349" t="s">
         <v>445</v>
       </c>
-      <c r="B49" s="355"/>
-      <c r="C49" s="355"/>
-      <c r="D49" s="355"/>
-      <c r="E49" s="355"/>
-      <c r="F49" s="355"/>
-      <c r="G49" s="355"/>
+      <c r="B49" s="349"/>
+      <c r="C49" s="349"/>
+      <c r="D49" s="349"/>
+      <c r="E49" s="349"/>
+      <c r="F49" s="349"/>
+      <c r="G49" s="349"/>
       <c r="I49" s="141" t="s">
         <v>444</v>
       </c>
@@ -22932,34 +22935,34 @@
       <c r="A67" s="151" t="s">
         <v>420</v>
       </c>
-      <c r="I67" s="364" t="s">
+      <c r="I67" s="354" t="s">
         <v>419</v>
       </c>
-      <c r="J67" s="364" t="s">
+      <c r="J67" s="354" t="s">
         <v>418</v>
       </c>
-      <c r="K67" s="365" t="s">
+      <c r="K67" s="355" t="s">
         <v>417</v>
       </c>
-      <c r="L67" s="366" t="s">
+      <c r="L67" s="351" t="s">
         <v>416</v>
       </c>
-      <c r="M67" s="353"/>
-      <c r="N67" s="353"/>
-      <c r="O67" s="366" t="s">
+      <c r="M67" s="350"/>
+      <c r="N67" s="350"/>
+      <c r="O67" s="351" t="s">
         <v>415</v>
       </c>
-      <c r="P67" s="353"/>
-      <c r="Q67" s="353"/>
-      <c r="R67" s="363" t="s">
+      <c r="P67" s="350"/>
+      <c r="Q67" s="350"/>
+      <c r="R67" s="353" t="s">
         <v>414</v>
       </c>
-      <c r="S67" s="363"/>
+      <c r="S67" s="353"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I68" s="364"/>
-      <c r="J68" s="364"/>
-      <c r="K68" s="365"/>
+      <c r="I68" s="354"/>
+      <c r="J68" s="354"/>
+      <c r="K68" s="355"/>
       <c r="L68" s="149">
         <v>2000</v>
       </c>
@@ -23636,14 +23639,14 @@
       <c r="I87" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="J87" s="370" t="s">
+      <c r="J87" s="352" t="s">
         <v>373</v>
       </c>
-      <c r="K87" s="370"/>
-      <c r="L87" s="370" t="s">
+      <c r="K87" s="352"/>
+      <c r="L87" s="352" t="s">
         <v>372</v>
       </c>
-      <c r="M87" s="370"/>
+      <c r="M87" s="352"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -24319,16 +24322,16 @@
       <c r="J123" s="113" t="s">
         <v>327</v>
       </c>
-      <c r="K123" s="367" t="s">
+      <c r="K123" s="346" t="s">
         <v>326</v>
       </c>
-      <c r="L123" s="368"/>
-      <c r="M123" s="369"/>
-      <c r="N123" s="367" t="s">
+      <c r="L123" s="347"/>
+      <c r="M123" s="348"/>
+      <c r="N123" s="346" t="s">
         <v>325</v>
       </c>
-      <c r="O123" s="368"/>
-      <c r="P123" s="369"/>
+      <c r="O123" s="347"/>
+      <c r="P123" s="348"/>
       <c r="Q123" s="114"/>
     </row>
     <row r="124" spans="9:17" x14ac:dyDescent="0.25">
@@ -24411,61 +24414,61 @@
       <c r="Q126" s="114"/>
     </row>
     <row r="128" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I128" s="355" t="s">
+      <c r="I128" s="349" t="s">
         <v>321</v>
       </c>
-      <c r="J128" s="355"/>
-      <c r="K128" s="355"/>
-      <c r="L128" s="355"/>
-      <c r="M128" s="355"/>
-      <c r="N128" s="355"/>
-      <c r="O128" s="355"/>
-      <c r="P128" s="355"/>
-      <c r="Q128" s="355"/>
+      <c r="J128" s="349"/>
+      <c r="K128" s="349"/>
+      <c r="L128" s="349"/>
+      <c r="M128" s="349"/>
+      <c r="N128" s="349"/>
+      <c r="O128" s="349"/>
+      <c r="P128" s="349"/>
+      <c r="Q128" s="349"/>
     </row>
     <row r="129" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I129" s="355"/>
-      <c r="J129" s="355"/>
-      <c r="K129" s="355"/>
-      <c r="L129" s="355"/>
-      <c r="M129" s="355"/>
-      <c r="N129" s="355"/>
-      <c r="O129" s="355"/>
-      <c r="P129" s="355"/>
-      <c r="Q129" s="355"/>
+      <c r="I129" s="349"/>
+      <c r="J129" s="349"/>
+      <c r="K129" s="349"/>
+      <c r="L129" s="349"/>
+      <c r="M129" s="349"/>
+      <c r="N129" s="349"/>
+      <c r="O129" s="349"/>
+      <c r="P129" s="349"/>
+      <c r="Q129" s="349"/>
     </row>
     <row r="130" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I130" s="355"/>
-      <c r="J130" s="355"/>
-      <c r="K130" s="355"/>
-      <c r="L130" s="355"/>
-      <c r="M130" s="355"/>
-      <c r="N130" s="355"/>
-      <c r="O130" s="355"/>
-      <c r="P130" s="355"/>
-      <c r="Q130" s="355"/>
+      <c r="I130" s="349"/>
+      <c r="J130" s="349"/>
+      <c r="K130" s="349"/>
+      <c r="L130" s="349"/>
+      <c r="M130" s="349"/>
+      <c r="N130" s="349"/>
+      <c r="O130" s="349"/>
+      <c r="P130" s="349"/>
+      <c r="Q130" s="349"/>
     </row>
     <row r="131" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I131" s="355"/>
-      <c r="J131" s="355"/>
-      <c r="K131" s="355"/>
-      <c r="L131" s="355"/>
-      <c r="M131" s="355"/>
-      <c r="N131" s="355"/>
-      <c r="O131" s="355"/>
-      <c r="P131" s="355"/>
-      <c r="Q131" s="355"/>
+      <c r="I131" s="349"/>
+      <c r="J131" s="349"/>
+      <c r="K131" s="349"/>
+      <c r="L131" s="349"/>
+      <c r="M131" s="349"/>
+      <c r="N131" s="349"/>
+      <c r="O131" s="349"/>
+      <c r="P131" s="349"/>
+      <c r="Q131" s="349"/>
     </row>
     <row r="132" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I132" s="355"/>
-      <c r="J132" s="355"/>
-      <c r="K132" s="355"/>
-      <c r="L132" s="355"/>
-      <c r="M132" s="355"/>
-      <c r="N132" s="355"/>
-      <c r="O132" s="355"/>
-      <c r="P132" s="355"/>
-      <c r="Q132" s="355"/>
+      <c r="I132" s="349"/>
+      <c r="J132" s="349"/>
+      <c r="K132" s="349"/>
+      <c r="L132" s="349"/>
+      <c r="M132" s="349"/>
+      <c r="N132" s="349"/>
+      <c r="O132" s="349"/>
+      <c r="P132" s="349"/>
+      <c r="Q132" s="349"/>
     </row>
     <row r="134" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I134" s="114" t="s">
@@ -24769,19 +24772,14 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="K123:M123"/>
-    <mergeCell ref="N123:P123"/>
-    <mergeCell ref="I128:Q132"/>
-    <mergeCell ref="R26:T26"/>
-    <mergeCell ref="O67:Q67"/>
-    <mergeCell ref="J87:K87"/>
-    <mergeCell ref="L87:M87"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="R67:S67"/>
-    <mergeCell ref="I67:I68"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="K67:K68"/>
-    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="O26:Q26"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L26:N26"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="L46:N46"/>
     <mergeCell ref="A49:G49"/>
@@ -24790,14 +24788,19 @@
     <mergeCell ref="D32:F32"/>
     <mergeCell ref="D33:F33"/>
     <mergeCell ref="D34:F34"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="K46:K47"/>
-    <mergeCell ref="O26:Q26"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="R67:S67"/>
+    <mergeCell ref="I67:I68"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="K67:K68"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="K123:M123"/>
+    <mergeCell ref="N123:P123"/>
+    <mergeCell ref="I128:Q132"/>
+    <mergeCell ref="R26:T26"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="J87:K87"/>
+    <mergeCell ref="L87:M87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" location="Hydrogen!A8" display="General Notes" xr:uid="{A141E675-9962-4785-8A8D-B1A687A4B1B7}"/>
@@ -32006,7 +32009,7 @@
   <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -32156,7 +32159,7 @@
         <v>837</v>
       </c>
       <c r="Y3" s="258" t="s">
-        <v>161</v>
+        <v>838</v>
       </c>
     </row>
     <row r="4" spans="1:31" ht="51" x14ac:dyDescent="0.2">

</xml_diff>